<commit_message>
add import by movie name
</commit_message>
<xml_diff>
--- a/docs/movies.xlsx
+++ b/docs/movies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/van/projects/likn/emdb/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194076F3-BB5C-B541-B491-91E3871B48BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6552F6B4-12D6-B647-8391-3562F2A2DB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-980" yWindow="-19400" windowWidth="30240" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companys" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="385">
   <si>
     <t>编号</t>
   </si>
@@ -1274,6 +1274,10 @@
   </si>
   <si>
     <t>BBC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>历史频道</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1626,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD51"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -3101,14 +3105,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
-      <c r="A135">
+    <row r="135" spans="1:3" s="4" customFormat="1" ht="17">
+      <c r="A135" s="4">
         <v>139</v>
       </c>
-      <c r="B135" t="s">
-        <v>135</v>
-      </c>
-      <c r="C135" t="s">
+      <c r="B135" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C135" s="4" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3446,8 +3450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add import tv script
</commit_message>
<xml_diff>
--- a/docs/movies.xlsx
+++ b/docs/movies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/van/projects/likn/emdb/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8626FDB9-5492-E64C-9642-CE98E697A343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A9AF2C-69A6-6142-B18D-CE2A0078174D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="-20600" windowWidth="30240" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-300" yWindow="-20600" windowWidth="30240" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companys" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="390">
   <si>
     <t>编号</t>
   </si>
@@ -1288,12 +1288,22 @@
     <t>DC Films</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>Marvel Studios</t>
+  </si>
+  <si>
+    <t>Kevin Feige Productions</t>
+  </si>
+  <si>
+    <t>Kevin Feige Productions</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1334,6 +1344,12 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1355,7 +1371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1371,6 +1387,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1646,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="B145" sqref="A1:C158"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="H134" sqref="H134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -3387,6 +3404,28 @@
         <v>386</v>
       </c>
     </row>
+    <row r="159" spans="1:3">
+      <c r="A159">
+        <v>163</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160">
+        <v>164</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>389</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3397,7 +3436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30E892-35C5-5F41-83CC-F6DF654C35B0}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update all tv_id rout
</commit_message>
<xml_diff>
--- a/docs/movies.xlsx
+++ b/docs/movies.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/van/projects/likn/emdb/docs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20251D1C-B9FA-404C-9F72-2D6E7AAA98FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="30240" windowHeight="17440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="30240" windowHeight="14900" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="companys" sheetId="1" r:id="rId1"/>
@@ -23,60 +17,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Wang, Emma</author>
-  </authors>
-  <commentList>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{B079A2BC-0DA2-764E-979C-77165990C464}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Wang, Emma:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">aka </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>迷雾追魂手</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="402">
   <si>
     <t>编号</t>
   </si>
@@ -546,14 +488,33 @@
     <t>优尼影视</t>
   </si>
   <si>
+    <t>儒意</t>
+  </si>
+  <si>
+    <t>Warner Bros. Pictures</t>
+  </si>
+  <si>
+    <t>DC Films</t>
+  </si>
+  <si>
+    <t>Marvel Studios</t>
+  </si>
+  <si>
+    <t>Kevin Feige Productions</t>
+  </si>
+  <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>movie_id(</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <rFont val="宋体-简"/>
-        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>影片编号</t>
@@ -562,20 +523,24 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>movie_name</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <rFont val="宋体-简"/>
-        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>（影片名称）</t>
@@ -583,13 +548,18 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
       <t>影片类型</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>1</t>
     </r>
@@ -597,7 +567,6 @@
       <rPr>
         <sz val="11"/>
         <rFont val="宋体-简"/>
-        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>：电影</t>
@@ -606,7 +575,7 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> 3</t>
     </r>
@@ -614,7 +583,6 @@
       <rPr>
         <sz val="11"/>
         <rFont val="宋体-简"/>
-        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>：季播剧</t>
@@ -622,13 +590,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>company_id</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <rFont val="宋体-简"/>
-        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>（版权公司编号）</t>
@@ -636,13 +608,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>copyright_start_time</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <rFont val="宋体-简"/>
-        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>（版权开始日期）</t>
@@ -650,13 +626,17 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>copyright_end_time</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <rFont val="宋体-简"/>
-        <family val="1"/>
         <charset val="134"/>
       </rPr>
       <t>（版权结束日期）</t>
@@ -1323,85 +1303,62 @@
     <t>2024-12-31 19:27:03</t>
   </si>
   <si>
-    <t>儒意</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>BBC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>历史频道</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Warner Bros. Pictures</t>
-  </si>
-  <si>
-    <t>DC Films</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Marvel Studios</t>
-  </si>
-  <si>
-    <t>Kevin Feige Productions</t>
-  </si>
-  <si>
-    <t>Kevin Feige Productions</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>墨水心</t>
-  </si>
-  <si>
-    <t>实习生</t>
-  </si>
-  <si>
-    <t>致命拜访</t>
-  </si>
-  <si>
-    <t>正义铁巨人</t>
-  </si>
-  <si>
-    <t>逃出克隆岛</t>
-  </si>
-  <si>
-    <t>西部英雄约拿·哈克斯</t>
-  </si>
-  <si>
-    <t>法官老爸</t>
-  </si>
-  <si>
-    <t>水中女妖</t>
-  </si>
-  <si>
-    <t>夜行人生</t>
-  </si>
-  <si>
-    <t>特工狂花</t>
-  </si>
-  <si>
-    <t>危机最前线</t>
-  </si>
-  <si>
-    <t>疯狂的麦克斯</t>
-  </si>
-  <si>
-    <t>疯狂的麦克斯2</t>
-  </si>
-  <si>
-    <t>疯狂的麦克斯3</t>
-  </si>
-  <si>
-    <t>疯狂的麦克斯：狂暴之路</t>
+    <t>哈利·波特与密室</t>
+  </si>
+  <si>
+    <t>哈利·波特与死亡圣器(上)</t>
+  </si>
+  <si>
+    <t>哈利·波特与死亡圣器(下)</t>
+  </si>
+  <si>
+    <t>哈利·波特与火焰杯</t>
+  </si>
+  <si>
+    <t>哈利·波特与混血王子</t>
+  </si>
+  <si>
+    <t>哈利·波特与凤凰社</t>
+  </si>
+  <si>
+    <t>哈利·波特与阿兹卡班的囚徒</t>
+  </si>
+  <si>
+    <t>哈利·波特与魔法石</t>
+  </si>
+  <si>
+    <t>躲藏</t>
+  </si>
+  <si>
+    <t>暴力史</t>
+  </si>
+  <si>
+    <t>我是传奇</t>
+  </si>
+  <si>
+    <t>我是山姆</t>
+  </si>
+  <si>
+    <t>海洋深处</t>
+  </si>
+  <si>
+    <t>超级魔术师</t>
+  </si>
+  <si>
+    <t>告密者</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1410,72 +1367,201 @@
     <font>
       <sz val="11"/>
       <name val="宋体-简"/>
-      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.8"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Microsoft YaHei"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF6A8759"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
+      <sz val="9.8"/>
       <color rgb="FFA9B7C6"/>
       <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1488,8 +1574,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1512,9 +1784,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1524,33 +2038,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1808,32 +2366,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C160"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="A22" sqref="$A22:$XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.3359375" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="16.8" spans="1:3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2046,7 +2604,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" customHeight="1">
+    <row r="21" ht="16" customHeight="1" spans="1:3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -2061,8 +2619,8 @@
       <c r="A22">
         <v>22</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>383</v>
+      <c r="B22" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -2992,7 +3550,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:2">
       <c r="A107">
         <v>111</v>
       </c>
@@ -3022,7 +3580,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:2">
       <c r="A110">
         <v>114</v>
       </c>
@@ -3030,7 +3588,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:2">
       <c r="A111">
         <v>115</v>
       </c>
@@ -3291,14 +3849,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="1:3" s="4" customFormat="1" ht="17">
-      <c r="A135" s="4">
+    <row r="135" s="5" customFormat="1" ht="14.4" spans="1:3">
+      <c r="A135" s="5">
         <v>139</v>
       </c>
-      <c r="B135" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="C135" s="4" t="s">
+      <c r="B135" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C135" s="5" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3522,15 +4080,15 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="1:3" s="4" customFormat="1" ht="17">
-      <c r="A156" s="4">
+    <row r="156" s="5" customFormat="1" ht="14.4" spans="1:3">
+      <c r="A156" s="5">
         <v>160</v>
       </c>
-      <c r="B156" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="C156" s="5" t="s">
-        <v>382</v>
+      <c r="B156" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C156" s="10" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -3538,10 +4096,10 @@
         <v>161</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>385</v>
+        <v>157</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>385</v>
+        <v>157</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3549,58 +4107,59 @@
         <v>162</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>386</v>
+        <v>158</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>386</v>
+        <v>158</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159">
         <v>163</v>
       </c>
-      <c r="B159" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="C159" s="9" t="s">
-        <v>387</v>
+      <c r="B159" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C159" s="11" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160">
         <v>164</v>
       </c>
-      <c r="B160" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="C160" s="6" t="s">
-        <v>389</v>
+      <c r="B160" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF30E892-35C5-5F41-83CC-F6DF654C35B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="16.8" spans="1:3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3609,10 +4168,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>385</v>
+        <v>157</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>385</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3620,36 +4179,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>386</v>
+        <v>158</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>386</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E559E5-A9BB-3D44-A273-65544BA4DBEF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="16.8" spans="1:3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3720,46 +4280,47 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="3" width="41.33203125" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" customWidth="1"/>
-    <col min="6" max="6" width="53.83203125" customWidth="1"/>
+    <col min="2" max="3" width="41.3359375" customWidth="1"/>
+    <col min="4" max="4" width="33.3359375" customWidth="1"/>
+    <col min="5" max="5" width="45.3359375" customWidth="1"/>
+    <col min="6" max="6" width="53.8359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" ht="17" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3767,7 +4328,7 @@
         <v>10009</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -3776,10 +4337,10 @@
         <v>85</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3787,7 +4348,7 @@
         <v>10022</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -3796,10 +4357,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3807,7 +4368,7 @@
         <v>10083</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -3816,10 +4377,10 @@
         <v>79</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3827,7 +4388,7 @@
         <v>10117</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -3836,10 +4397,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3847,7 +4408,7 @@
         <v>10161</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -3856,10 +4417,10 @@
         <v>94</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3867,7 +4428,7 @@
         <v>10174</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -3876,10 +4437,10 @@
         <v>102</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3887,7 +4448,7 @@
         <v>10190</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -3896,10 +4457,10 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3907,7 +4468,7 @@
         <v>10222</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -3916,10 +4477,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3927,7 +4488,7 @@
         <v>10225</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -3936,10 +4497,10 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3947,7 +4508,7 @@
         <v>10226</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -3956,10 +4517,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3967,7 +4528,7 @@
         <v>10227</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -3976,10 +4537,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3987,7 +4548,7 @@
         <v>10231</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -3996,10 +4557,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -4007,7 +4568,7 @@
         <v>10232</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -4016,10 +4577,10 @@
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4027,7 +4588,7 @@
         <v>10236</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -4036,10 +4597,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -4047,7 +4608,7 @@
         <v>10239</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -4056,10 +4617,10 @@
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -4067,7 +4628,7 @@
         <v>10266</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -4076,10 +4637,10 @@
         <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4087,7 +4648,7 @@
         <v>10300</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -4096,10 +4657,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -4107,7 +4668,7 @@
         <v>10399</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -4116,10 +4677,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4127,7 +4688,7 @@
         <v>10427</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -4136,10 +4697,10 @@
         <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4147,7 +4708,7 @@
         <v>10430</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -4156,10 +4717,10 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4167,7 +4728,7 @@
         <v>10453</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -4176,10 +4737,10 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -4187,7 +4748,7 @@
         <v>10454</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -4196,10 +4757,10 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -4207,7 +4768,7 @@
         <v>10463</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -4216,10 +4777,10 @@
         <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4227,7 +4788,7 @@
         <v>10592</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -4236,10 +4797,10 @@
         <v>149</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4247,7 +4808,7 @@
         <v>10595</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -4256,10 +4817,10 @@
         <v>6</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -4267,7 +4828,7 @@
         <v>10607</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -4276,10 +4837,10 @@
         <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -4287,7 +4848,7 @@
         <v>10646</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -4296,10 +4857,10 @@
         <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -4307,7 +4868,7 @@
         <v>10649</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -4316,10 +4877,10 @@
         <v>5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4327,7 +4888,7 @@
         <v>10650</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -4336,30 +4897,30 @@
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="4" customFormat="1">
-      <c r="A31" s="7">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" s="5" customFormat="1" spans="1:6">
+      <c r="A31" s="6">
         <v>10686</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C31" s="7">
+      <c r="B31" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>149</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>221</v>
+      <c r="E31" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4367,7 +4928,7 @@
         <v>10734</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -4376,10 +4937,10 @@
         <v>146</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4387,7 +4948,7 @@
         <v>10735</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -4396,10 +4957,10 @@
         <v>2</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -4407,7 +4968,7 @@
         <v>10737</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -4416,10 +4977,10 @@
         <v>118</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4427,7 +4988,7 @@
         <v>10738</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
@@ -4436,10 +4997,10 @@
         <v>118</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -4447,7 +5008,7 @@
         <v>10758</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -4456,10 +5017,10 @@
         <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4467,7 +5028,7 @@
         <v>10768</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -4476,10 +5037,10 @@
         <v>6</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4487,7 +5048,7 @@
         <v>10772</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
@@ -4496,10 +5057,10 @@
         <v>146</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -4507,7 +5068,7 @@
         <v>10776</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
@@ -4516,10 +5077,10 @@
         <v>149</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -4527,7 +5088,7 @@
         <v>10791</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
@@ -4536,10 +5097,10 @@
         <v>2</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -4547,7 +5108,7 @@
         <v>10793</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
@@ -4556,10 +5117,10 @@
         <v>2</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -4567,7 +5128,7 @@
         <v>10820</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
@@ -4576,10 +5137,10 @@
         <v>6</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -4587,7 +5148,7 @@
         <v>10824</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
@@ -4596,10 +5157,10 @@
         <v>149</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -4607,7 +5168,7 @@
         <v>10826</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
@@ -4616,10 +5177,10 @@
         <v>5</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -4627,7 +5188,7 @@
         <v>10828</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
@@ -4636,10 +5197,10 @@
         <v>6</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -4647,7 +5208,7 @@
         <v>10838</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
@@ -4656,10 +5217,10 @@
         <v>2</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4667,7 +5228,7 @@
         <v>10857</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C47" s="1">
         <v>1</v>
@@ -4676,10 +5237,10 @@
         <v>2</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -4687,7 +5248,7 @@
         <v>10868</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
@@ -4696,10 +5257,10 @@
         <v>149</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -4707,7 +5268,7 @@
         <v>10877</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
@@ -4716,10 +5277,10 @@
         <v>2</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -4727,7 +5288,7 @@
         <v>10930</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
@@ -4736,10 +5297,10 @@
         <v>149</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -4747,7 +5308,7 @@
         <v>11105</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
@@ -4756,10 +5317,10 @@
         <v>149</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -4767,7 +5328,7 @@
         <v>11117</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
@@ -4776,10 +5337,10 @@
         <v>2</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -4787,7 +5348,7 @@
         <v>11123</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C53" s="1">
         <v>1</v>
@@ -4796,10 +5357,10 @@
         <v>2</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -4807,7 +5368,7 @@
         <v>11125</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
@@ -4816,10 +5377,10 @@
         <v>5</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -4827,7 +5388,7 @@
         <v>11159</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
@@ -4836,10 +5397,10 @@
         <v>146</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -4847,7 +5408,7 @@
         <v>11196</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="C56" s="1">
         <v>1</v>
@@ -4856,10 +5417,10 @@
         <v>146</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -4867,7 +5428,7 @@
         <v>11203</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C57" s="1">
         <v>1</v>
@@ -4876,10 +5437,10 @@
         <v>2</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -4887,7 +5448,7 @@
         <v>11208</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
@@ -4896,10 +5457,10 @@
         <v>5</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -4907,7 +5468,7 @@
         <v>11250</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
@@ -4916,10 +5477,10 @@
         <v>118</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -4927,7 +5488,7 @@
         <v>11252</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
@@ -4936,10 +5497,10 @@
         <v>118</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -4947,7 +5508,7 @@
         <v>11253</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C61" s="1">
         <v>1</v>
@@ -4956,10 +5517,10 @@
         <v>118</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -4967,7 +5528,7 @@
         <v>11884</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C62" s="1">
         <v>3</v>
@@ -4976,10 +5537,10 @@
         <v>124</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -4987,7 +5548,7 @@
         <v>12254</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="C63" s="1">
         <v>3</v>
@@ -4996,10 +5557,10 @@
         <v>118</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -5007,7 +5568,7 @@
         <v>15222</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C64" s="1">
         <v>3</v>
@@ -5016,10 +5577,10 @@
         <v>122</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -5027,7 +5588,7 @@
         <v>19065</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="C65" s="1">
         <v>3</v>
@@ -5036,10 +5597,10 @@
         <v>2</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -5047,7 +5608,7 @@
         <v>20959</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C66" s="1">
         <v>3</v>
@@ -5056,10 +5617,10 @@
         <v>122</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -5067,7 +5628,7 @@
         <v>26539</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C67" s="1">
         <v>3</v>
@@ -5076,10 +5637,10 @@
         <v>122</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -5087,7 +5648,7 @@
         <v>34284</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C68" s="1">
         <v>3</v>
@@ -5096,10 +5657,10 @@
         <v>122</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -5107,7 +5668,7 @@
         <v>36717</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C69" s="1">
         <v>3</v>
@@ -5116,10 +5677,10 @@
         <v>122</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -5127,7 +5688,7 @@
         <v>37426</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C70" s="1">
         <v>3</v>
@@ -5136,10 +5697,10 @@
         <v>122</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -5147,7 +5708,7 @@
         <v>37678</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C71" s="1">
         <v>3</v>
@@ -5156,10 +5717,10 @@
         <v>122</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -5167,7 +5728,7 @@
         <v>38345</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="C72" s="1">
         <v>3</v>
@@ -5176,10 +5737,10 @@
         <v>122</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -5187,7 +5748,7 @@
         <v>38455</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C73" s="1">
         <v>3</v>
@@ -5196,10 +5757,10 @@
         <v>122</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -5207,7 +5768,7 @@
         <v>38695</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C74" s="1">
         <v>3</v>
@@ -5216,10 +5777,10 @@
         <v>122</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -5227,7 +5788,7 @@
         <v>38732</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C75" s="1">
         <v>3</v>
@@ -5236,10 +5797,10 @@
         <v>122</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -5247,7 +5808,7 @@
         <v>38865</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C76" s="1">
         <v>3</v>
@@ -5256,10 +5817,10 @@
         <v>122</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -5267,7 +5828,7 @@
         <v>39709</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C77" s="1">
         <v>3</v>
@@ -5276,10 +5837,10 @@
         <v>122</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -5287,7 +5848,7 @@
         <v>39743</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="C78" s="1">
         <v>3</v>
@@ -5296,10 +5857,10 @@
         <v>122</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -5307,7 +5868,7 @@
         <v>41443</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="C79" s="1">
         <v>3</v>
@@ -5316,10 +5877,10 @@
         <v>122</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -5327,7 +5888,7 @@
         <v>47125</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C80" s="1">
         <v>3</v>
@@ -5336,10 +5897,10 @@
         <v>150</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -5347,7 +5908,7 @@
         <v>47259</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="C81" s="1">
         <v>3</v>
@@ -5356,10 +5917,10 @@
         <v>150</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -5367,7 +5928,7 @@
         <v>47572</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="C82" s="1">
         <v>3</v>
@@ -5376,10 +5937,10 @@
         <v>150</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -5387,7 +5948,7 @@
         <v>47618</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="C83" s="1">
         <v>3</v>
@@ -5396,10 +5957,10 @@
         <v>150</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -5407,7 +5968,7 @@
         <v>47678</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="C84" s="1">
         <v>3</v>
@@ -5416,10 +5977,10 @@
         <v>150</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -5427,7 +5988,7 @@
         <v>48183</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C85" s="1">
         <v>3</v>
@@ -5436,10 +5997,10 @@
         <v>22</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -5447,7 +6008,7 @@
         <v>48303</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C86" s="1">
         <v>3</v>
@@ -5456,10 +6017,10 @@
         <v>150</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -5467,7 +6028,7 @@
         <v>48365</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C87" s="1">
         <v>3</v>
@@ -5476,10 +6037,10 @@
         <v>150</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -5487,7 +6048,7 @@
         <v>48565</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C88" s="1">
         <v>3</v>
@@ -5496,10 +6057,10 @@
         <v>150</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -5507,7 +6068,7 @@
         <v>48816</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C89" s="1">
         <v>3</v>
@@ -5516,10 +6077,10 @@
         <v>150</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -5527,7 +6088,7 @@
         <v>48864</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="C90" s="1">
         <v>3</v>
@@ -5536,10 +6097,10 @@
         <v>150</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -5547,7 +6108,7 @@
         <v>48919</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C91" s="1">
         <v>3</v>
@@ -5556,10 +6117,10 @@
         <v>150</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -5567,7 +6128,7 @@
         <v>48955</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C92" s="1">
         <v>3</v>
@@ -5576,10 +6137,10 @@
         <v>150</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -5587,7 +6148,7 @@
         <v>49009</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="C93" s="1">
         <v>3</v>
@@ -5596,10 +6157,10 @@
         <v>150</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -5607,7 +6168,7 @@
         <v>49039</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="C94" s="1">
         <v>3</v>
@@ -5616,10 +6177,10 @@
         <v>150</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -5627,7 +6188,7 @@
         <v>49071</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="C95" s="1">
         <v>3</v>
@@ -5636,10 +6197,10 @@
         <v>150</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -5647,7 +6208,7 @@
         <v>49551</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="C96" s="1">
         <v>3</v>
@@ -5656,10 +6217,10 @@
         <v>2</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -5667,7 +6228,7 @@
         <v>50038</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="C97" s="1">
         <v>3</v>
@@ -5676,10 +6237,10 @@
         <v>150</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -5687,7 +6248,7 @@
         <v>51577</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="C98" s="1">
         <v>3</v>
@@ -5696,10 +6257,10 @@
         <v>150</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -5707,7 +6268,7 @@
         <v>51835</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="C99" s="1">
         <v>3</v>
@@ -5716,10 +6277,10 @@
         <v>150</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -5727,7 +6288,7 @@
         <v>52026</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C100" s="1">
         <v>3</v>
@@ -5736,10 +6297,10 @@
         <v>150</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -5747,7 +6308,7 @@
         <v>52459</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="C101" s="1">
         <v>3</v>
@@ -5756,126 +6317,126 @@
         <v>150</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD9342B1-AE64-AC44-A0A5-64C84AC7BDFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="32.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="32.8359375" defaultRowHeight="14" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" ht="17" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="B2" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" ht="14.4" spans="2:2">
+      <c r="B2" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" ht="14.4" spans="2:2">
+      <c r="B3" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" ht="14.4" spans="2:2">
+      <c r="B4" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="5" ht="14.4" spans="2:2">
+      <c r="B5" s="3" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="B3" s="11" t="s">
+    <row r="6" ht="14.4" spans="2:2">
+      <c r="B6" s="3" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="B4" s="11" t="s">
+    <row r="7" ht="14.4" spans="2:2">
+      <c r="B7" s="3" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="B5" s="11" t="s">
+    <row r="8" ht="14.4" spans="2:2">
+      <c r="B8" s="3" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="B6" s="11" t="s">
+    <row r="9" ht="14.4" spans="2:2">
+      <c r="B9" s="3" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="11" t="s">
+    <row r="10" ht="14.4" spans="2:2">
+      <c r="B10" s="4" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="11" t="s">
+    <row r="11" ht="14.4" spans="2:2">
+      <c r="B11" s="4" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="11" t="s">
+    <row r="12" ht="14.4" spans="2:2">
+      <c r="B12" s="3" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="B10" s="11" t="s">
+    <row r="13" ht="14.4" spans="2:2">
+      <c r="B13" s="4" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="B11" s="11" t="s">
+    <row r="14" ht="14.4" spans="2:2">
+      <c r="B14" s="4" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="B12" s="11" t="s">
+    <row r="15" ht="14.4" spans="2:2">
+      <c r="B15" s="4" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="B13" s="11" t="s">
+    <row r="16" ht="14.4" spans="2:2">
+      <c r="B16" s="4" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="B14" s="11" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="B15" s="11" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="10" t="s">
-        <v>404</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update movie_info when exist
</commit_message>
<xml_diff>
--- a/docs/movies.xlsx
+++ b/docs/movies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14220" activeTab="4"/>
+    <workbookView windowWidth="30240" windowHeight="14220" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="companys" sheetId="1" r:id="rId1"/>
@@ -1543,8 +1543,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -1605,7 +1605,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1620,10 +1620,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1642,9 +1643,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1658,25 +1667,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1690,29 +1682,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1722,6 +1691,37 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1749,7 +1749,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1761,13 +1869,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1779,13 +1911,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1797,133 +1923,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1934,6 +1934,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1963,9 +1972,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1999,57 +2034,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2058,103 +2058,103 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2163,22 +2163,22 @@
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2521,8 +2521,8 @@
   <sheetPr/>
   <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B17"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -6481,8 +6481,8 @@
   <sheetPr/>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.8359375" defaultRowHeight="14" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
update movies' name for search english name
</commit_message>
<xml_diff>
--- a/docs/movies.xlsx
+++ b/docs/movies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="14220" activeTab="4"/>
+    <workbookView windowHeight="14220" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="companys" sheetId="1" r:id="rId1"/>
@@ -1429,28 +1429,28 @@
     <t>浴血无名·奔袭</t>
   </si>
   <si>
-    <t>调职到乐队！</t>
-  </si>
-  <si>
-    <t>幸存者</t>
-  </si>
-  <si>
-    <t>末日协议</t>
-  </si>
-  <si>
-    <t>行骗天下英雄篇</t>
-  </si>
-  <si>
-    <t>罪恶围城</t>
-  </si>
-  <si>
-    <t>埋葬</t>
-  </si>
-  <si>
-    <t>第一座奥斯卡</t>
-  </si>
-  <si>
-    <t>承包商</t>
+    <t>Offbeat Cops</t>
+  </si>
+  <si>
+    <t>The Survivor</t>
+  </si>
+  <si>
+    <t>The Deal</t>
+  </si>
+  <si>
+    <t>The Confidence Man JP: Episode of the Hero</t>
+  </si>
+  <si>
+    <t>BAD CITY</t>
+  </si>
+  <si>
+    <t>Burial</t>
+  </si>
+  <si>
+    <t>First Oscar</t>
+  </si>
+  <si>
+    <t>The Contractor</t>
   </si>
   <si>
     <t>穿墙之弹 （穿墙而行）</t>
@@ -1486,13 +1486,13 @@
     <t>勇闯16街区</t>
   </si>
   <si>
-    <t>同床异客</t>
-  </si>
-  <si>
-    <t>德维塔耶夫</t>
-  </si>
-  <si>
-    <t>老亨利</t>
+    <t>The Stranger in Our Bed</t>
+  </si>
+  <si>
+    <t>V2 Escape from Hell</t>
+  </si>
+  <si>
+    <t>Old Henry</t>
   </si>
   <si>
     <t>致命感应</t>
@@ -1507,34 +1507,34 @@
     <t>黑夜传说</t>
   </si>
   <si>
-    <t>降灵日历</t>
-  </si>
-  <si>
-    <t>不洁净的血</t>
-  </si>
-  <si>
-    <t>逆时杀机</t>
-  </si>
-  <si>
-    <t>黑夜侵蚀世界</t>
-  </si>
-  <si>
-    <t>杀人镜头</t>
-  </si>
-  <si>
-    <t>绑架/失踪的男孩</t>
-  </si>
-  <si>
-    <t>危险止痛</t>
-  </si>
-  <si>
-    <t>狩猎季节</t>
-  </si>
-  <si>
-    <t>呼吸</t>
-  </si>
-  <si>
-    <t>痕迹</t>
+    <t>The Advent Calendar</t>
+  </si>
+  <si>
+    <t>The Breitner Commando</t>
+  </si>
+  <si>
+    <t>Silencio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Night Eats the World</t>
+  </si>
+  <si>
+    <t>Murder in the Lens</t>
+  </si>
+  <si>
+    <t>Boy Missing/Secuestro</t>
+  </si>
+  <si>
+    <t>Painkillers</t>
+  </si>
+  <si>
+    <t>Hunting Season</t>
+  </si>
+  <si>
+    <t>Last Breath</t>
+  </si>
+  <si>
+    <t>The Trace</t>
   </si>
 </sst>
 </file>
@@ -1543,9 +1543,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1591,7 +1591,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1599,6 +1614,52 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1612,9 +1673,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1622,6 +1682,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1629,7 +1705,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1644,14 +1720,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -1659,76 +1727,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1749,18 +1749,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1773,7 +1761,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1785,127 +1785,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1923,7 +1803,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1940,8 +1940,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1951,6 +1966,45 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1980,205 +2034,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -6481,8 +6481,8 @@
   <sheetPr/>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.8359375" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -7075,19 +7075,19 @@
         <v>457</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" ht="16.8" spans="1:2">
       <c r="A73">
         <v>457955</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="5" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" ht="16.8" spans="1:2">
       <c r="A74">
         <v>527004</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="5" t="s">
         <v>459</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add update season/epsodes method
</commit_message>
<xml_diff>
--- a/docs/movies.xlsx
+++ b/docs/movies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="14900" activeTab="4"/>
+    <workbookView windowWidth="30240" windowHeight="14900" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="companys" sheetId="1" r:id="rId1"/>
@@ -6931,7 +6931,7 @@
   <sheetPr/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6995,8 +6995,8 @@
   <sheetPr/>
   <dimension ref="A1:V640"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -7028,7 +7028,7 @@
     </row>
     <row r="2" ht="16.8" spans="1:22">
       <c r="A2">
-        <v>52814</v>
+        <v>202065</v>
       </c>
       <c r="B2" t="s">
         <v>391</v>

</xml_diff>

<commit_message>
add update used tv season
</commit_message>
<xml_diff>
--- a/docs/movies.xlsx
+++ b/docs/movies.xlsx
@@ -1314,9 +1314,6 @@
   </si>
   <si>
     <t>凯伦·皮里 第二季</t>
-  </si>
-  <si>
-    <t>光环 第一季</t>
   </si>
   <si>
     <t>塔楼 第三季</t>
@@ -1588,19 +1585,10 @@
     <t>不眠 第二季</t>
   </si>
   <si>
-    <t>黄蜂 第一季</t>
-  </si>
-  <si>
     <t>洪水之后</t>
   </si>
   <si>
-    <t>那时那处</t>
-  </si>
-  <si>
     <t>迷失海湾 第五季</t>
-  </si>
-  <si>
-    <t>奇妙人生</t>
   </si>
   <si>
     <r>
@@ -1718,124 +1706,136 @@
     <t>格雷斯 第四季</t>
   </si>
   <si>
+    <t>194636, 126167, 87773, 227496, 47224,295144</t>
+  </si>
+  <si>
+    <t>迪莉娅的证词（原：直到我杀了你）</t>
+  </si>
+  <si>
+    <t>格雷斯 第三季</t>
+  </si>
+  <si>
+    <t>渎职</t>
+  </si>
+  <si>
+    <t>探案拍档 第四季</t>
+  </si>
+  <si>
+    <t>光环 第一季</t>
+  </si>
+  <si>
+    <t>设得兰谜案 第七季</t>
+  </si>
+  <si>
+    <t>黄蜂 第一季</t>
+  </si>
+  <si>
+    <t>山巅之城 第三季</t>
+  </si>
+  <si>
+    <t>那时那处</t>
+  </si>
+  <si>
+    <t>仁医莎姆</t>
+  </si>
+  <si>
+    <t>奇妙人生</t>
+  </si>
+  <si>
+    <t>超蓬勃：优步之战 第一季</t>
+  </si>
+  <si>
     <t>英伦魔法师</t>
   </si>
   <si>
-    <t>194636, 126167, 87773, 227496, 47224,295144</t>
-  </si>
-  <si>
-    <t>迪莉娅的证词（原：直到我杀了你）</t>
+    <t>法官大人 第二季</t>
   </si>
   <si>
     <t>安妮日记</t>
   </si>
   <si>
-    <t>格雷斯 第三季</t>
-  </si>
-  <si>
     <t>贝奥武夫</t>
   </si>
   <si>
-    <t>渎职</t>
-  </si>
-  <si>
     <t>化身博士</t>
   </si>
   <si>
-    <t>探案拍档 第四季</t>
+    <t>说出你的秘密</t>
   </si>
   <si>
     <t>黑暗天使</t>
   </si>
   <si>
-    <t>设得兰谜案 第七季</t>
+    <t>山巅之城 第二季</t>
   </si>
   <si>
     <t>海豹六队 第一季</t>
   </si>
   <si>
+    <t>新阴阳魔界 第二季</t>
+  </si>
+  <si>
     <t>弗兰肯斯坦传奇 第一季</t>
   </si>
   <si>
-    <t>山巅之城 第三季</t>
+    <t>波尔达克 第五季</t>
   </si>
   <si>
     <t>罪恶的灵魂 第一季</t>
   </si>
   <si>
-    <t>仁医莎姆</t>
+    <t>重任在肩S5</t>
   </si>
   <si>
     <t>罪恶的灵魂 第二季</t>
   </si>
   <si>
-    <t>超蓬勃：优步之战 第一季</t>
+    <t>山巅之城 第一季</t>
   </si>
   <si>
     <t>塞尔福里奇先生 第一季</t>
   </si>
   <si>
-    <t>法官大人 第二季</t>
+    <t>韦恩 第一季</t>
   </si>
   <si>
     <t>塞尔福里奇先生 第二季</t>
   </si>
   <si>
+    <t>莱姆镇</t>
+  </si>
+  <si>
     <t>塞尔福里奇先生 第三季</t>
   </si>
   <si>
+    <t>新阴阳魔界 第一季</t>
+  </si>
+  <si>
     <t>塞尔福里奇先生 第四季</t>
   </si>
   <si>
-    <t>说出你的秘密</t>
+    <t>波尔达克 第四季</t>
   </si>
   <si>
     <t>重任在肩S1</t>
   </si>
   <si>
-    <t>山巅之城 第二季</t>
+    <t>海豹六队 第二季</t>
   </si>
   <si>
     <t>重任在肩S2</t>
   </si>
   <si>
-    <t>新阴阳魔界 第二季</t>
+    <t>波尔达克 第三季</t>
   </si>
   <si>
     <t>重任在肩S4</t>
   </si>
   <si>
-    <t>波尔达克 第五季</t>
-  </si>
-  <si>
     <t>波尔达克 第一季</t>
   </si>
   <si>
-    <t>重任在肩S5</t>
-  </si>
-  <si>
     <t>波尔达克 第二季</t>
-  </si>
-  <si>
-    <t>山巅之城 第一季</t>
-  </si>
-  <si>
-    <t>波尔达克 第三季</t>
-  </si>
-  <si>
-    <t>韦恩 第一季</t>
-  </si>
-  <si>
-    <t>波尔达克 第四季</t>
-  </si>
-  <si>
-    <t>莱姆镇</t>
-  </si>
-  <si>
-    <t>新阴阳魔界 第一季</t>
-  </si>
-  <si>
-    <t>海豹六队 第二季</t>
   </si>
   <si>
     <t>弗兰肯斯坦传奇 第二季</t>
@@ -1965,6 +1965,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <color rgb="FFF8F8F2"/>
       <name val="Monaco"/>
@@ -1974,13 +1981,6 @@
       <sz val="11"/>
       <name val="宋体-简"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2493,13 +2493,13 @@
     <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2559,13 +2559,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2583,7 +2583,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2598,7 +2598,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2629,18 +2629,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2982,13 +2982,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="16.8" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4750,13 +4750,13 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" ht="16.8" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4800,13 +4800,13 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" ht="16.8" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -6993,10 +6993,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V640"/>
+  <dimension ref="A1:P640"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -7006,7 +7006,7 @@
     <col min="13" max="13" width="19.40625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:22">
+    <row r="1" ht="16.8" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>387</v>
       </c>
@@ -7016,1353 +7016,1184 @@
       <c r="C1" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="T1" s="8">
+    </row>
+    <row r="2" ht="16.8" spans="1:3">
+      <c r="A2" s="4">
         <v>194636</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="V1" s="7">
+      <c r="C2" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="16.8" spans="1:22">
-      <c r="A2">
+    <row r="3" ht="16.8" spans="1:6">
+      <c r="A3" s="4">
+        <v>138181</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" ht="16.8" spans="1:3">
+      <c r="A4" s="4">
+        <v>126167</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" ht="16.8" spans="1:3">
+      <c r="A5" s="4">
+        <v>241097</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="17" spans="1:16">
+      <c r="A6" s="4">
+        <v>87773</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="7" ht="16.8" spans="1:9">
+      <c r="A7" s="4">
+        <v>120317</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" ht="16.8" spans="1:3">
+      <c r="A8" s="4">
+        <v>227496</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="16.8" spans="1:3">
+      <c r="A9" s="4">
+        <v>120317</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" ht="16.8" spans="1:3">
+      <c r="A10" s="4">
+        <v>223389</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="16.8" spans="1:15">
+      <c r="A11" s="4">
+        <v>99962</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4</v>
+      </c>
+      <c r="M11">
         <v>202065</v>
       </c>
-      <c r="B2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="T2" s="8">
-        <v>138181</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="V2" s="7">
+      <c r="N11" t="s">
+        <v>409</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="16.8" spans="1:15">
+      <c r="A12" s="4">
+        <v>46923</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="C12" s="5">
+        <v>7</v>
+      </c>
+      <c r="M12">
+        <v>118357</v>
+      </c>
+      <c r="N12">
+        <v>1883</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="16.8" spans="1:15">
+      <c r="A13" s="4">
+        <v>52814</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>117488</v>
+      </c>
+      <c r="N13" t="s">
+        <v>411</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" ht="16.8" spans="1:15">
+      <c r="A14" s="4">
+        <v>79618</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="C14" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" ht="16.8" spans="1:22">
-      <c r="A3">
+      <c r="M14">
+        <v>70390</v>
+      </c>
+      <c r="N14" t="s">
+        <v>413</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" ht="16.8" spans="1:15">
+      <c r="A15" s="4">
+        <v>125952</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>295144</v>
+      </c>
+      <c r="N15" t="s">
+        <v>415</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" ht="16.8" spans="1:15">
+      <c r="A16" s="4">
+        <v>126301</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>62717</v>
+      </c>
+      <c r="N16" t="s">
+        <v>417</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" ht="16.8" spans="1:15">
+      <c r="A17" s="4">
+        <v>86430</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>28379</v>
+      </c>
+      <c r="N17" t="s">
+        <v>419</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" ht="16.8" spans="1:15">
+      <c r="A18" s="4">
         <v>118357</v>
       </c>
-      <c r="B3">
+      <c r="B18" s="5">
         <v>1883</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="T3" s="8">
-        <v>126167</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="V3" s="7">
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>64593</v>
+      </c>
+      <c r="N18" t="s">
+        <v>420</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" ht="16.8" spans="1:15">
+      <c r="A19" s="4">
+        <v>117488</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>47224</v>
+      </c>
+      <c r="N19" t="s">
+        <v>421</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" ht="16.8" spans="1:15">
+      <c r="A20" s="4">
+        <v>90452</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>67961</v>
+      </c>
+      <c r="N20" t="s">
+        <v>423</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" ht="16.8" spans="1:15">
+      <c r="A21" s="4">
+        <v>79618</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="C21" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" ht="16.8" spans="1:22">
-      <c r="A4">
-        <v>117488</v>
-      </c>
-      <c r="B4" t="s">
-        <v>395</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="T4" s="8">
-        <v>241097</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="V4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" ht="16.8" spans="1:22">
-      <c r="A5">
+      <c r="M21">
+        <v>66871</v>
+      </c>
+      <c r="N21" t="s">
+        <v>425</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" ht="16.8" spans="1:15">
+      <c r="A22" s="4">
+        <v>83135</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>64421</v>
+      </c>
+      <c r="N22" t="s">
+        <v>427</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" ht="16.8" spans="1:15">
+      <c r="A23" s="4">
+        <v>62084</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
+      <c r="M23">
+        <v>61239</v>
+      </c>
+      <c r="N23" t="s">
+        <v>429</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" ht="16.8" spans="1:15">
+      <c r="A24" s="4">
+        <v>43982</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <v>61239</v>
+      </c>
+      <c r="N24" t="s">
+        <v>431</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" ht="16.8" spans="1:15">
+      <c r="A25" s="4">
+        <v>79618</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>46643</v>
+      </c>
+      <c r="N25" t="s">
+        <v>433</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" ht="16.8" spans="1:15">
+      <c r="A26" s="4">
+        <v>84231</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>46643</v>
+      </c>
+      <c r="N26" t="s">
+        <v>435</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" ht="16.8" spans="1:15">
+      <c r="A27" s="4">
+        <v>90254</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>46643</v>
+      </c>
+      <c r="N27" t="s">
+        <v>437</v>
+      </c>
+      <c r="O27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" ht="16.8" spans="1:15">
+      <c r="A28" s="4">
+        <v>83135</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>46643</v>
+      </c>
+      <c r="N28" t="s">
+        <v>439</v>
+      </c>
+      <c r="O28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" ht="16.8" spans="1:15">
+      <c r="A29" s="4">
+        <v>62084</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="C29" s="5">
+        <v>4</v>
+      </c>
+      <c r="M29">
+        <v>43982</v>
+      </c>
+      <c r="N29" t="s">
+        <v>441</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" ht="16.8" spans="1:15">
+      <c r="A30" s="4">
+        <v>66871</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2</v>
+      </c>
+      <c r="M30">
+        <v>43982</v>
+      </c>
+      <c r="N30" t="s">
+        <v>443</v>
+      </c>
+      <c r="O30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" ht="16.8" spans="1:15">
+      <c r="A31" s="4">
+        <v>62084</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C31" s="5">
+        <v>3</v>
+      </c>
+      <c r="M31">
+        <v>43982</v>
+      </c>
+      <c r="N31" t="s">
+        <v>445</v>
+      </c>
+      <c r="O31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" ht="16.8" spans="1:15">
+      <c r="A32" s="4">
         <v>70390</v>
       </c>
-      <c r="B5" t="s">
-        <v>397</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="T5" s="8">
-        <v>87773</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="V5" s="7">
+      <c r="B32" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>62084</v>
+      </c>
+      <c r="N32" t="s">
+        <v>446</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" ht="16.8" spans="1:15">
+      <c r="A33" s="4">
+        <v>66871</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>62084</v>
+      </c>
+      <c r="N33" t="s">
+        <v>447</v>
+      </c>
+      <c r="O33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" ht="16.8" spans="1:15">
+      <c r="A34" s="4">
+        <v>43982</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="C34" s="5">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>62084</v>
+      </c>
+      <c r="N34" t="s">
+        <v>444</v>
+      </c>
+      <c r="O34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" ht="16.8" spans="1:15">
+      <c r="A35" s="4">
+        <v>64421</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>62084</v>
+      </c>
+      <c r="N35" t="s">
+        <v>440</v>
+      </c>
+      <c r="O35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" ht="16.8" spans="1:15">
+      <c r="A36" s="4">
+        <v>62425</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="C36" s="5">
+        <v>3</v>
+      </c>
+      <c r="M36">
+        <v>62084</v>
+      </c>
+      <c r="N36" t="s">
+        <v>428</v>
+      </c>
+      <c r="O36">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="17" spans="1:22">
-      <c r="A6">
-        <v>295144</v>
-      </c>
-      <c r="B6" t="s">
-        <v>399</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="T6" s="8">
-        <v>120317</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="V6" s="7">
+    <row r="37" ht="16.8" spans="1:3">
+      <c r="A37" s="4">
+        <v>56336</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="C37" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" ht="16.8" spans="1:3">
+      <c r="A38" s="4">
+        <v>61239</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="C38" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" ht="16.8" spans="1:3">
+      <c r="A39" s="4">
+        <v>64593</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" ht="16.8" spans="1:3">
+      <c r="A40" s="4">
+        <v>46643</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="C40" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="7" ht="16.8" spans="1:22">
-      <c r="A7">
+    <row r="41" ht="16.8" spans="1:3">
+      <c r="A41" s="4">
+        <v>62084</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" ht="16.8" spans="1:3">
+      <c r="A42" s="4">
+        <v>43982</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="C42" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" ht="16.8" spans="1:3">
+      <c r="A43" s="4">
+        <v>62425</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C43" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" ht="16.8" spans="1:3">
+      <c r="A44" s="4">
+        <v>56336</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C44" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" ht="16.8" spans="1:3">
+      <c r="A45" s="4">
+        <v>61239</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="C45" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" ht="16.8" spans="1:3">
+      <c r="A46" s="4">
+        <v>47224</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="C46" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" ht="16.8" spans="1:3">
+      <c r="A47" s="4">
+        <v>46643</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C47" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" ht="16.8" spans="1:3">
+      <c r="A48" s="4">
+        <v>62084</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C48" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" ht="16.8" spans="1:3">
+      <c r="A49" s="4">
+        <v>67961</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" ht="16.8" spans="1:3">
+      <c r="A50" s="4">
+        <v>64421</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" ht="16.8" spans="1:3">
+      <c r="A51" s="4">
+        <v>49010</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C51" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" ht="16.8" spans="1:3">
+      <c r="A52" s="4">
+        <v>62208</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C52" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" ht="16.8" spans="1:3">
+      <c r="A53" s="4">
+        <v>43020</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C53" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" ht="16.8" spans="1:3">
+      <c r="A54" s="4">
+        <v>62425</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" ht="16.8" spans="1:3">
+      <c r="A55" s="4">
+        <v>46643</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C55" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" ht="16.8" spans="1:3">
+      <c r="A56" s="4">
+        <v>43982</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C56" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" ht="16.8" spans="1:3">
+      <c r="A57" s="4">
+        <v>49010</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C57" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" ht="16.8" spans="1:3">
+      <c r="A58" s="4">
+        <v>46746</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="C58" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" ht="16.8" spans="1:3">
+      <c r="A59" s="4">
+        <v>46511</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C59" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" ht="16.8" spans="1:3">
+      <c r="A60" s="4">
+        <v>46643</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C60" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" ht="16.8" spans="1:3">
+      <c r="A61" s="4">
         <v>62717</v>
       </c>
-      <c r="B7" t="s">
-        <v>408</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>409</v>
-      </c>
-      <c r="T7" s="8">
-        <v>227496</v>
-      </c>
-      <c r="U7" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="V7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="16.8" spans="1:22">
-      <c r="A8">
+      <c r="B61" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="C61" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" ht="16.8" spans="1:3">
+      <c r="A62" s="4">
+        <v>56484</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" ht="16.8" spans="1:3">
+      <c r="A63" s="4">
+        <v>49010</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="C63" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" ht="16.8" spans="1:3">
+      <c r="A64" s="4">
+        <v>46746</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" ht="16.8" spans="1:3">
+      <c r="A65" s="4">
+        <v>46511</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="C65" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" ht="16.8" spans="1:3">
+      <c r="A66" s="4">
+        <v>43020</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="C66" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" ht="16.8" spans="1:3">
+      <c r="A67" s="4">
+        <v>56336</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="C67" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" ht="16.8" spans="1:3">
+      <c r="A68" s="4">
+        <v>43982</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="C68" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" ht="16.8" spans="1:3">
+      <c r="A69" s="4">
+        <v>39718</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="C69" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" ht="16.8" spans="1:3">
+      <c r="A70" s="4">
+        <v>43020</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="C70" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" ht="16.8" spans="1:3">
+      <c r="A71" s="4">
+        <v>43020</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="C71" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" ht="16.8" spans="1:3">
+      <c r="A72" s="4">
+        <v>39718</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C72" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" ht="16.8" spans="1:3">
+      <c r="A73" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="C73" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" ht="16.8" spans="1:3">
+      <c r="A74" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="C74" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" ht="16.8" spans="1:3">
+      <c r="A75" s="4">
         <v>28379</v>
       </c>
-      <c r="B8" t="s">
-        <v>411</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="T8" s="8">
-        <v>120317</v>
-      </c>
-      <c r="U8" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="V8" s="7">
+      <c r="B75" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" ht="16.8" spans="1:3">
+      <c r="A76" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="C76" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" ht="16.8" spans="1:3">
+      <c r="A77" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C77" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" ht="16.8" spans="1:3">
+      <c r="A78" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="C78" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" ht="16.8" spans="1:3">
+      <c r="A79" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="C79" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" ht="16.8" spans="1:3">
+      <c r="A80" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="C80" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" ht="16.8" spans="1:3">
+      <c r="A81" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C81" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="9" ht="16.8" spans="1:22">
-      <c r="A9">
-        <v>64593</v>
-      </c>
-      <c r="B9" t="s">
-        <v>413</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="T9" s="8">
-        <v>223389</v>
-      </c>
-      <c r="U9" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="V9" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" ht="16.8" spans="1:22">
-      <c r="A10">
-        <v>47224</v>
-      </c>
-      <c r="B10" t="s">
-        <v>415</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="T10" s="8">
-        <v>99962</v>
-      </c>
-      <c r="U10" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="V10" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" ht="16.8" spans="1:22">
-      <c r="A11">
-        <v>67961</v>
-      </c>
-      <c r="B11" t="s">
-        <v>417</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="T11" s="8">
-        <v>46923</v>
-      </c>
-      <c r="U11" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="V11" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" ht="16.8" spans="1:22">
-      <c r="A12">
-        <v>66871</v>
-      </c>
-      <c r="B12" t="s">
-        <v>419</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="T12" s="8">
-        <v>52814</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="V12" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" ht="16.8" spans="1:22">
-      <c r="A13">
-        <v>64421</v>
-      </c>
-      <c r="B13" t="s">
-        <v>420</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="T13" s="8">
-        <v>79618</v>
-      </c>
-      <c r="U13" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="V13" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" ht="16.8" spans="1:22">
-      <c r="A14">
-        <v>61239</v>
-      </c>
-      <c r="B14" t="s">
-        <v>422</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="T14" s="8">
-        <v>125952</v>
-      </c>
-      <c r="U14" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="V14" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" ht="16.8" spans="1:22">
-      <c r="A15">
-        <v>61239</v>
-      </c>
-      <c r="B15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C15">
+    <row r="82" ht="16.8" spans="1:3">
+      <c r="A82" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="C82" s="5">
         <v>2</v>
       </c>
-      <c r="T15" s="8">
-        <v>126301</v>
-      </c>
-      <c r="U15" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="V15" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" ht="16.8" spans="1:22">
-      <c r="A16">
-        <v>46643</v>
-      </c>
-      <c r="B16" t="s">
-        <v>426</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="T16" s="8">
-        <v>86430</v>
-      </c>
-      <c r="U16" s="7" t="s">
-        <v>427</v>
-      </c>
-      <c r="V16" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" ht="16.8" spans="1:22">
-      <c r="A17">
-        <v>46643</v>
-      </c>
-      <c r="B17" t="s">
-        <v>428</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="T17" s="8">
-        <v>118357</v>
-      </c>
-      <c r="U17" s="7">
-        <v>1883</v>
-      </c>
-      <c r="V17" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" ht="16.8" spans="1:22">
-      <c r="A18">
-        <v>46643</v>
-      </c>
-      <c r="B18" t="s">
-        <v>429</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="T18" s="8">
-        <v>117488</v>
-      </c>
-      <c r="U18" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="V18" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" ht="16.8" spans="1:22">
-      <c r="A19">
-        <v>46643</v>
-      </c>
-      <c r="B19" t="s">
-        <v>430</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="T19" s="8">
-        <v>90452</v>
-      </c>
-      <c r="U19" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="V19" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" ht="16.8" spans="1:22">
-      <c r="A20">
-        <v>43982</v>
-      </c>
-      <c r="B20" t="s">
-        <v>432</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="T20" s="8">
-        <v>79618</v>
-      </c>
-      <c r="U20" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="V20" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" ht="16.8" spans="1:22">
-      <c r="A21">
-        <v>43982</v>
-      </c>
-      <c r="B21" t="s">
-        <v>434</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="T21" s="8">
-        <v>83135</v>
-      </c>
-      <c r="U21" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="V21" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" ht="16.8" spans="1:22">
-      <c r="A22">
-        <v>43982</v>
-      </c>
-      <c r="B22" t="s">
-        <v>436</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="T22" s="8">
-        <v>62084</v>
-      </c>
-      <c r="U22" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="V22" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" ht="16.8" spans="1:22">
-      <c r="A23">
-        <v>62084</v>
-      </c>
-      <c r="B23" t="s">
-        <v>438</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="T23" s="8">
-        <v>43982</v>
-      </c>
-      <c r="U23" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="V23" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" ht="16.8" spans="1:22">
-      <c r="A24">
-        <v>62084</v>
-      </c>
-      <c r="B24" t="s">
-        <v>440</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="T24" s="8">
-        <v>79618</v>
-      </c>
-      <c r="U24" s="7" t="s">
-        <v>441</v>
-      </c>
-      <c r="V24" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" ht="16.8" spans="1:22">
-      <c r="A25">
-        <v>62084</v>
-      </c>
-      <c r="B25" t="s">
-        <v>442</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="T25" s="8">
-        <v>84231</v>
-      </c>
-      <c r="U25" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="V25" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" ht="16.8" spans="1:22">
-      <c r="A26">
-        <v>62084</v>
-      </c>
-      <c r="B26" t="s">
-        <v>444</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="T26" s="8">
-        <v>90254</v>
-      </c>
-      <c r="U26" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="V26" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" ht="16.8" spans="1:22">
-      <c r="A27">
-        <v>62084</v>
-      </c>
-      <c r="B27" t="s">
-        <v>437</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-      <c r="T27" s="8">
-        <v>83135</v>
-      </c>
-      <c r="U27" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="V27" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" ht="16.8" spans="1:22">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="T28" s="8">
-        <v>62084</v>
-      </c>
-      <c r="U28" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="V28" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" ht="16.8" spans="1:22">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="T29" s="8">
-        <v>66871</v>
-      </c>
-      <c r="U29" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="V29" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" ht="16.8" spans="1:22">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="T30" s="8">
-        <v>62084</v>
-      </c>
-      <c r="U30" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="V30" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" ht="16.8" spans="1:22">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="T31" s="8">
-        <v>70390</v>
-      </c>
-      <c r="U31" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="V31" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" ht="16.8" spans="1:22">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="T32" s="8">
-        <v>66871</v>
-      </c>
-      <c r="U32" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="V32" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" ht="16.8" spans="1:22">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="T33" s="8">
-        <v>43982</v>
-      </c>
-      <c r="U33" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="V33" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" ht="16.8" spans="1:22">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="T34" s="8">
-        <v>64421</v>
-      </c>
-      <c r="U34" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="V34" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" ht="16.8" spans="1:22">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="T35" s="8">
-        <v>62425</v>
-      </c>
-      <c r="U35" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="V35" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" ht="16.8" spans="1:22">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="T36" s="8">
-        <v>56336</v>
-      </c>
-      <c r="U36" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="V36" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" ht="16.8" spans="1:22">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="T37" s="8">
-        <v>61239</v>
-      </c>
-      <c r="U37" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="V37" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" ht="16.8" spans="1:22">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="T38" s="8">
-        <v>64593</v>
-      </c>
-      <c r="U38" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="V38" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" ht="16.8" spans="1:22">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="T39" s="8">
-        <v>46643</v>
-      </c>
-      <c r="U39" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="V39" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" ht="16.8" spans="1:22">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="T40" s="8">
-        <v>62084</v>
-      </c>
-      <c r="U40" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="V40" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" ht="16.8" spans="1:22">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="T41" s="8">
-        <v>43982</v>
-      </c>
-      <c r="U41" s="7" t="s">
-        <v>451</v>
-      </c>
-      <c r="V41" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" ht="16.8" spans="1:22">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="T42" s="8">
-        <v>62425</v>
-      </c>
-      <c r="U42" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="V42" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" ht="16.8" spans="1:22">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="T43" s="8">
-        <v>56336</v>
-      </c>
-      <c r="U43" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="V43" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" ht="16.8" spans="1:22">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="T44" s="8">
-        <v>61239</v>
-      </c>
-      <c r="U44" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="V44" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" ht="16.8" spans="1:22">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="T45" s="8">
-        <v>47224</v>
-      </c>
-      <c r="U45" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="V45" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" ht="16.8" spans="1:22">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="T46" s="8">
-        <v>46643</v>
-      </c>
-      <c r="U46" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="V46" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" ht="16.8" spans="1:22">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="T47" s="8">
-        <v>62084</v>
-      </c>
-      <c r="U47" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="V47" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" ht="16.8" spans="1:22">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="T48" s="8">
-        <v>67961</v>
-      </c>
-      <c r="U48" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="V48" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" ht="16.8" spans="1:22">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="T49" s="8">
-        <v>64421</v>
-      </c>
-      <c r="U49" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="V49" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" ht="16.8" spans="1:22">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="T50" s="8">
-        <v>49010</v>
-      </c>
-      <c r="U50" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="V50" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" ht="16.8" spans="1:22">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="T51" s="8">
-        <v>62208</v>
-      </c>
-      <c r="U51" s="7" t="s">
-        <v>455</v>
-      </c>
-      <c r="V51" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" ht="16.8" spans="1:22">
-      <c r="A52"/>
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="T52" s="8">
-        <v>43020</v>
-      </c>
-      <c r="U52" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="V52" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" ht="16.8" spans="1:22">
-      <c r="A53"/>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="T53" s="8">
-        <v>62425</v>
-      </c>
-      <c r="U53" s="7" t="s">
-        <v>457</v>
-      </c>
-      <c r="V53" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" ht="16.8" spans="1:22">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="T54" s="8">
-        <v>46643</v>
-      </c>
-      <c r="U54" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="V54" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" ht="16.8" spans="1:22">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="T55" s="8">
-        <v>43982</v>
-      </c>
-      <c r="U55" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="V55" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" ht="16.8" spans="1:22">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="T56" s="8">
-        <v>49010</v>
-      </c>
-      <c r="U56" s="7" t="s">
-        <v>458</v>
-      </c>
-      <c r="V56" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" ht="16.8" spans="1:22">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57"/>
-      <c r="T57" s="8">
-        <v>46746</v>
-      </c>
-      <c r="U57" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="V57" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" ht="16.8" spans="1:22">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="T58" s="8">
-        <v>46511</v>
-      </c>
-      <c r="U58" s="7" t="s">
-        <v>460</v>
-      </c>
-      <c r="V58" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" ht="16.8" spans="1:22">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="T59" s="8">
-        <v>46643</v>
-      </c>
-      <c r="U59" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="V59" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" ht="16.8" spans="1:22">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="T60" s="8">
-        <v>62717</v>
-      </c>
-      <c r="U60" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="V60" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" ht="16.8" spans="1:22">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="T61" s="8">
-        <v>56484</v>
-      </c>
-      <c r="U61" s="7" t="s">
-        <v>461</v>
-      </c>
-      <c r="V61" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" ht="16.8" spans="1:22">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="T62" s="8">
-        <v>49010</v>
-      </c>
-      <c r="U62" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="V62" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" ht="16.8" spans="1:22">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="T63" s="8">
-        <v>46746</v>
-      </c>
-      <c r="U63" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="V63" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" ht="16.8" spans="1:22">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="T64" s="8">
-        <v>46511</v>
-      </c>
-      <c r="U64" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="V64" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" ht="16.8" spans="1:22">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="T65" s="8">
-        <v>43020</v>
-      </c>
-      <c r="U65" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="V65" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" ht="16.8" spans="1:22">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="T66" s="8">
-        <v>56336</v>
-      </c>
-      <c r="U66" s="7" t="s">
-        <v>466</v>
-      </c>
-      <c r="V66" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" ht="16.8" spans="1:22">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="T67" s="8">
-        <v>43982</v>
-      </c>
-      <c r="U67" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="V67" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" ht="16.8" spans="1:22">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="T68" s="8">
+    </row>
+    <row r="83" ht="16.8" spans="1:3">
+      <c r="A83" s="4">
+        <v>4046</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C83" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" ht="16.8" spans="1:3">
+      <c r="A84" s="9">
         <v>39718</v>
       </c>
-      <c r="U68" s="7" t="s">
+      <c r="B84" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="V68" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" ht="16.8" spans="1:22">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="T69" s="8">
-        <v>43020</v>
-      </c>
-      <c r="U69" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="V69" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" ht="16.8" spans="1:22">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="T70" s="8">
-        <v>43020</v>
-      </c>
-      <c r="U70" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="V70" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" ht="16.8" spans="1:22">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="T71" s="8">
-        <v>39718</v>
-      </c>
-      <c r="U71" s="7" t="s">
-        <v>470</v>
-      </c>
-      <c r="V71" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" ht="16.8" spans="1:22">
-      <c r="A72"/>
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="T72" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U72" s="7" t="s">
-        <v>471</v>
-      </c>
-      <c r="V72" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" ht="16.8" spans="1:22">
-      <c r="A73"/>
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="T73" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U73" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="V73" s="7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" ht="16.8" spans="1:22">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
-      <c r="T74" s="8">
-        <v>28379</v>
-      </c>
-      <c r="U74" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="V74" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" ht="16.8" spans="1:22">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75"/>
-      <c r="T75" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U75" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="V75" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" ht="16.8" spans="1:22">
-      <c r="A76"/>
-      <c r="B76"/>
-      <c r="C76"/>
-      <c r="T76" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U76" s="7" t="s">
-        <v>474</v>
-      </c>
-      <c r="V76" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" ht="16.8" spans="1:22">
-      <c r="A77"/>
-      <c r="B77"/>
-      <c r="C77"/>
-      <c r="T77" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U77" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="V77" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" ht="16.8" spans="1:22">
-      <c r="A78"/>
-      <c r="B78"/>
-      <c r="C78"/>
-      <c r="T78" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U78" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="V78" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" ht="16.8" spans="1:22">
-      <c r="A79"/>
-      <c r="B79"/>
-      <c r="C79"/>
-      <c r="T79" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U79" s="7" t="s">
-        <v>477</v>
-      </c>
-      <c r="V79" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" ht="16.8" spans="1:22">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="T80" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U80" s="7" t="s">
-        <v>478</v>
-      </c>
-      <c r="V80" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" ht="16.8" spans="1:22">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="T81" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U81" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="V81" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" ht="16.8" spans="1:22">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="T82" s="8">
-        <v>4046</v>
-      </c>
-      <c r="U82" s="7" t="s">
-        <v>480</v>
-      </c>
-      <c r="V82" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" ht="16.8" spans="1:22">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-      <c r="T83" s="9">
-        <v>39718</v>
-      </c>
-      <c r="U83" s="9" t="s">
-        <v>467</v>
-      </c>
-      <c r="V83" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84"/>
+      <c r="C84" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="85" ht="16.8" spans="1:15">
       <c r="A85"/>
-      <c r="O85" s="5" t="s">
+      <c r="O85" s="7" t="s">
         <v>481</v>
       </c>
     </row>
@@ -10032,9 +9863,6 @@
       <c r="A640"/>
     </row>
   </sheetData>
-  <sortState ref="A86:A614">
-    <sortCondition ref="A82"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
add update used tv season2
</commit_message>
<xml_diff>
--- a/docs/movies.xlsx
+++ b/docs/movies.xlsx
@@ -2620,7 +2620,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2629,7 +2629,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2982,13 +2981,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="16.8" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4446,14 +4445,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" s="12" customFormat="1" ht="14.4" spans="1:3">
-      <c r="A135" s="12">
+    <row r="135" s="11" customFormat="1" ht="14.4" spans="1:3">
+      <c r="A135" s="11">
         <v>139</v>
       </c>
-      <c r="B135" s="15" t="s">
+      <c r="B135" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C135" s="12" t="s">
+      <c r="C135" s="11" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4677,14 +4676,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156" s="12" customFormat="1" ht="14.4" spans="1:3">
-      <c r="A156" s="12">
+    <row r="156" s="11" customFormat="1" ht="14.4" spans="1:3">
+      <c r="A156" s="11">
         <v>160</v>
       </c>
-      <c r="B156" s="15" t="s">
+      <c r="B156" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C156" s="15" t="s">
+      <c r="C156" s="14" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4692,10 +4691,10 @@
       <c r="A157">
         <v>161</v>
       </c>
-      <c r="B157" s="14" t="s">
+      <c r="B157" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C157" s="14" t="s">
+      <c r="C157" s="13" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4703,10 +4702,10 @@
       <c r="A158">
         <v>162</v>
       </c>
-      <c r="B158" s="14" t="s">
+      <c r="B158" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C158" s="14" t="s">
+      <c r="C158" s="13" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4714,10 +4713,10 @@
       <c r="A159">
         <v>163</v>
       </c>
-      <c r="B159" s="16" t="s">
+      <c r="B159" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C159" s="16" t="s">
+      <c r="C159" s="15" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4725,7 +4724,7 @@
       <c r="A160">
         <v>164</v>
       </c>
-      <c r="B160" s="16" t="s">
+      <c r="B160" s="15" t="s">
         <v>160</v>
       </c>
       <c r="C160" t="s">
@@ -4750,13 +4749,13 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" ht="16.8" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4764,10 +4763,10 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4775,10 +4774,10 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4800,13 +4799,13 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" ht="16.8" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4901,2022 +4900,2022 @@
   </cols>
   <sheetData>
     <row r="1" ht="17" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>10009</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="10">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10">
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9">
         <v>85</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>10022</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>10083</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="10">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
         <v>79</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>10117</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="10">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>10161</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9">
         <v>94</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>10174</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="10">
-        <v>1</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
         <v>102</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>10190</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="10">
-        <v>1</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>10222</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="10">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
         <v>2</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>10225</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10">
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
         <v>2</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>10226</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="10">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9">
         <v>2</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>10227</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="10">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>10231</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C13" s="10">
-        <v>1</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
         <v>2</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>10232</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C14" s="10">
-        <v>1</v>
-      </c>
-      <c r="D14" s="10">
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9">
         <v>2</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>10236</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C15" s="10">
-        <v>1</v>
-      </c>
-      <c r="D15" s="10">
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
         <v>2</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>10239</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C16" s="10">
-        <v>1</v>
-      </c>
-      <c r="D16" s="10">
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9">
         <v>2</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>10266</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C17" s="10">
-        <v>1</v>
-      </c>
-      <c r="D17" s="10">
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9">
         <v>5</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <v>10300</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C18" s="10">
-        <v>1</v>
-      </c>
-      <c r="D18" s="10">
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9">
         <v>2</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>10399</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="10">
-        <v>1</v>
-      </c>
-      <c r="D19" s="10">
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" s="9">
         <v>2</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>10427</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C20" s="10">
-        <v>1</v>
-      </c>
-      <c r="D20" s="10">
+      <c r="C20" s="9">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9">
         <v>5</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>10430</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C21" s="10">
-        <v>1</v>
-      </c>
-      <c r="D21" s="10">
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9">
         <v>2</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>10453</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C22" s="10">
-        <v>1</v>
-      </c>
-      <c r="D22" s="10">
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+      <c r="D22" s="9">
         <v>2</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>10454</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="10">
-        <v>1</v>
-      </c>
-      <c r="D23" s="10">
+      <c r="C23" s="9">
+        <v>1</v>
+      </c>
+      <c r="D23" s="9">
         <v>2</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>10463</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="C24" s="10">
-        <v>1</v>
-      </c>
-      <c r="D24" s="10">
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="9">
         <v>5</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>10592</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C25" s="10">
-        <v>1</v>
-      </c>
-      <c r="D25" s="10">
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9">
         <v>149</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>10595</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C26" s="10">
-        <v>1</v>
-      </c>
-      <c r="D26" s="10">
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
+      <c r="D26" s="9">
         <v>6</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <v>10607</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C27" s="10">
-        <v>1</v>
-      </c>
-      <c r="D27" s="10">
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9">
         <v>5</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>10646</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C28" s="10">
-        <v>1</v>
-      </c>
-      <c r="D28" s="10">
+      <c r="C28" s="9">
+        <v>1</v>
+      </c>
+      <c r="D28" s="9">
         <v>13</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>10649</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C29" s="10">
-        <v>1</v>
-      </c>
-      <c r="D29" s="10">
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9">
         <v>5</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <v>10650</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C30" s="10">
-        <v>1</v>
-      </c>
-      <c r="D30" s="10">
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30" s="9">
         <v>5</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="9" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="31" s="12" customFormat="1" spans="1:6">
-      <c r="A31" s="13">
+    <row r="31" s="11" customFormat="1" spans="1:6">
+      <c r="A31" s="12">
         <v>10686</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C31" s="13">
-        <v>1</v>
-      </c>
-      <c r="D31" s="13">
+      <c r="C31" s="12">
+        <v>1</v>
+      </c>
+      <c r="D31" s="12">
         <v>149</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="12" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="10">
+      <c r="A32" s="9">
         <v>10734</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C32" s="10">
-        <v>1</v>
-      </c>
-      <c r="D32" s="10">
+      <c r="C32" s="9">
+        <v>1</v>
+      </c>
+      <c r="D32" s="9">
         <v>146</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="9" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>10735</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C33" s="10">
-        <v>1</v>
-      </c>
-      <c r="D33" s="10">
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33" s="9">
         <v>2</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="10">
+      <c r="A34" s="9">
         <v>10737</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="C34" s="10">
-        <v>1</v>
-      </c>
-      <c r="D34" s="10">
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34" s="9">
         <v>118</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="9" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="10">
+      <c r="A35" s="9">
         <v>10738</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C35" s="10">
-        <v>1</v>
-      </c>
-      <c r="D35" s="10">
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="D35" s="9">
         <v>118</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="9" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="10">
+      <c r="A36" s="9">
         <v>10758</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="C36" s="10">
-        <v>1</v>
-      </c>
-      <c r="D36" s="10">
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9">
         <v>2</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="10">
+      <c r="A37" s="9">
         <v>10768</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C37" s="10">
-        <v>1</v>
-      </c>
-      <c r="D37" s="10">
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+      <c r="D37" s="9">
         <v>6</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="9" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="10">
+      <c r="A38" s="9">
         <v>10772</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="C38" s="10">
-        <v>1</v>
-      </c>
-      <c r="D38" s="10">
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="D38" s="9">
         <v>146</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="9" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="10">
+      <c r="A39" s="9">
         <v>10776</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C39" s="10">
-        <v>1</v>
-      </c>
-      <c r="D39" s="10">
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+      <c r="D39" s="9">
         <v>149</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="9" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="10">
+      <c r="A40" s="9">
         <v>10791</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="C40" s="10">
-        <v>1</v>
-      </c>
-      <c r="D40" s="10">
+      <c r="C40" s="9">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9">
         <v>2</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="10">
+      <c r="A41" s="9">
         <v>10793</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="C41" s="10">
-        <v>1</v>
-      </c>
-      <c r="D41" s="10">
+      <c r="C41" s="9">
+        <v>1</v>
+      </c>
+      <c r="D41" s="9">
         <v>2</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="10">
+      <c r="A42" s="9">
         <v>10820</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C42" s="10">
-        <v>1</v>
-      </c>
-      <c r="D42" s="10">
+      <c r="C42" s="9">
+        <v>1</v>
+      </c>
+      <c r="D42" s="9">
         <v>6</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="9" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="10">
+      <c r="A43" s="9">
         <v>10824</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C43" s="10">
-        <v>1</v>
-      </c>
-      <c r="D43" s="10">
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="D43" s="9">
         <v>149</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="9" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="10">
+      <c r="A44" s="9">
         <v>10826</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="C44" s="10">
-        <v>1</v>
-      </c>
-      <c r="D44" s="10">
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="9">
         <v>5</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="9" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="10">
+      <c r="A45" s="9">
         <v>10828</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C45" s="10">
-        <v>1</v>
-      </c>
-      <c r="D45" s="10">
+      <c r="C45" s="9">
+        <v>1</v>
+      </c>
+      <c r="D45" s="9">
         <v>6</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="9" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="10">
+      <c r="A46" s="9">
         <v>10838</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="C46" s="10">
-        <v>1</v>
-      </c>
-      <c r="D46" s="10">
+      <c r="C46" s="9">
+        <v>1</v>
+      </c>
+      <c r="D46" s="9">
         <v>2</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="10">
+      <c r="A47" s="9">
         <v>10857</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="C47" s="10">
-        <v>1</v>
-      </c>
-      <c r="D47" s="10">
+      <c r="C47" s="9">
+        <v>1</v>
+      </c>
+      <c r="D47" s="9">
         <v>2</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="10">
+      <c r="A48" s="9">
         <v>10868</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="C48" s="10">
-        <v>1</v>
-      </c>
-      <c r="D48" s="10">
+      <c r="C48" s="9">
+        <v>1</v>
+      </c>
+      <c r="D48" s="9">
         <v>149</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="9" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="10">
+      <c r="A49" s="9">
         <v>10877</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="C49" s="10">
-        <v>1</v>
-      </c>
-      <c r="D49" s="10">
+      <c r="C49" s="9">
+        <v>1</v>
+      </c>
+      <c r="D49" s="9">
         <v>2</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="10">
+      <c r="A50" s="9">
         <v>10930</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="C50" s="10">
-        <v>1</v>
-      </c>
-      <c r="D50" s="10">
+      <c r="C50" s="9">
+        <v>1</v>
+      </c>
+      <c r="D50" s="9">
         <v>149</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="9" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="10">
+      <c r="A51" s="9">
         <v>11105</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="C51" s="10">
-        <v>1</v>
-      </c>
-      <c r="D51" s="10">
+      <c r="C51" s="9">
+        <v>1</v>
+      </c>
+      <c r="D51" s="9">
         <v>149</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="9" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="10">
+      <c r="A52" s="9">
         <v>11117</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="C52" s="10">
-        <v>1</v>
-      </c>
-      <c r="D52" s="10">
+      <c r="C52" s="9">
+        <v>1</v>
+      </c>
+      <c r="D52" s="9">
         <v>2</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="10">
+      <c r="A53" s="9">
         <v>11123</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="C53" s="10">
-        <v>1</v>
-      </c>
-      <c r="D53" s="10">
+      <c r="C53" s="9">
+        <v>1</v>
+      </c>
+      <c r="D53" s="9">
         <v>2</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="10">
+      <c r="A54" s="9">
         <v>11125</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="C54" s="10">
-        <v>1</v>
-      </c>
-      <c r="D54" s="10">
+      <c r="C54" s="9">
+        <v>1</v>
+      </c>
+      <c r="D54" s="9">
         <v>5</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="9" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="10">
+      <c r="A55" s="9">
         <v>11159</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="C55" s="10">
-        <v>1</v>
-      </c>
-      <c r="D55" s="10">
+      <c r="C55" s="9">
+        <v>1</v>
+      </c>
+      <c r="D55" s="9">
         <v>146</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F55" s="9" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="10">
+      <c r="A56" s="9">
         <v>11196</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="C56" s="10">
-        <v>1</v>
-      </c>
-      <c r="D56" s="10">
+      <c r="C56" s="9">
+        <v>1</v>
+      </c>
+      <c r="D56" s="9">
         <v>146</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="9" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="10">
+      <c r="A57" s="9">
         <v>11203</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C57" s="10">
-        <v>1</v>
-      </c>
-      <c r="D57" s="10">
+      <c r="C57" s="9">
+        <v>1</v>
+      </c>
+      <c r="D57" s="9">
         <v>2</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="10">
+      <c r="A58" s="9">
         <v>11208</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="C58" s="10">
-        <v>1</v>
-      </c>
-      <c r="D58" s="10">
+      <c r="C58" s="9">
+        <v>1</v>
+      </c>
+      <c r="D58" s="9">
         <v>5</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="F58" s="9" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="10">
+      <c r="A59" s="9">
         <v>11250</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C59" s="10">
-        <v>1</v>
-      </c>
-      <c r="D59" s="10">
+      <c r="C59" s="9">
+        <v>1</v>
+      </c>
+      <c r="D59" s="9">
         <v>118</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="F59" s="10" t="s">
+      <c r="F59" s="9" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="10">
+      <c r="A60" s="9">
         <v>11252</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="C60" s="10">
-        <v>1</v>
-      </c>
-      <c r="D60" s="10">
+      <c r="C60" s="9">
+        <v>1</v>
+      </c>
+      <c r="D60" s="9">
         <v>118</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="E60" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="F60" s="10" t="s">
+      <c r="F60" s="9" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="10">
+      <c r="A61" s="9">
         <v>11253</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C61" s="10">
-        <v>1</v>
-      </c>
-      <c r="D61" s="10">
+      <c r="C61" s="9">
+        <v>1</v>
+      </c>
+      <c r="D61" s="9">
         <v>118</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="E61" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F61" s="9" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="10">
+      <c r="A62" s="9">
         <v>11884</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="9">
         <v>3</v>
       </c>
-      <c r="D62" s="10">
+      <c r="D62" s="9">
         <v>124</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E62" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="F62" s="10" t="s">
+      <c r="F62" s="9" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="10">
+      <c r="A63" s="9">
         <v>12254</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="9">
         <v>3</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="9">
         <v>118</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="F63" s="10" t="s">
+      <c r="F63" s="9" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="10">
+      <c r="A64" s="9">
         <v>15222</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="9">
         <v>3</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="9">
         <v>122</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="E64" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F64" s="10" t="s">
+      <c r="F64" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="10">
+      <c r="A65" s="9">
         <v>19065</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="9">
         <v>3</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="9">
         <v>2</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E65" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="10">
+      <c r="A66" s="9">
         <v>20959</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="9">
         <v>3</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="9">
         <v>122</v>
       </c>
-      <c r="E66" s="10" t="s">
+      <c r="E66" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="F66" s="10" t="s">
+      <c r="F66" s="9" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="10">
+      <c r="A67" s="9">
         <v>26539</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="9">
         <v>3</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D67" s="9">
         <v>122</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="E67" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F67" s="10" t="s">
+      <c r="F67" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="10">
+      <c r="A68" s="9">
         <v>34284</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="9">
         <v>3</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="9">
         <v>122</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E68" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F68" s="10" t="s">
+      <c r="F68" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="10">
+      <c r="A69" s="9">
         <v>36717</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B69" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="9">
         <v>3</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="9">
         <v>122</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E69" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="F69" s="9" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="10">
+      <c r="A70" s="9">
         <v>37426</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="9">
         <v>3</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D70" s="9">
         <v>122</v>
       </c>
-      <c r="E70" s="10" t="s">
+      <c r="E70" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="F70" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="10">
+      <c r="A71" s="9">
         <v>37678</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B71" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C71" s="9">
         <v>3</v>
       </c>
-      <c r="D71" s="10">
+      <c r="D71" s="9">
         <v>122</v>
       </c>
-      <c r="E71" s="10" t="s">
+      <c r="E71" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F71" s="10" t="s">
+      <c r="F71" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="10">
+      <c r="A72" s="9">
         <v>38345</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="C72" s="10">
+      <c r="C72" s="9">
         <v>3</v>
       </c>
-      <c r="D72" s="10">
+      <c r="D72" s="9">
         <v>122</v>
       </c>
-      <c r="E72" s="10" t="s">
+      <c r="E72" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F72" s="10" t="s">
+      <c r="F72" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="10">
+      <c r="A73" s="9">
         <v>38455</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B73" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="C73" s="10">
+      <c r="C73" s="9">
         <v>3</v>
       </c>
-      <c r="D73" s="10">
+      <c r="D73" s="9">
         <v>122</v>
       </c>
-      <c r="E73" s="10" t="s">
+      <c r="E73" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F73" s="10" t="s">
+      <c r="F73" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="10">
+      <c r="A74" s="9">
         <v>38695</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C74" s="9">
         <v>3</v>
       </c>
-      <c r="D74" s="10">
+      <c r="D74" s="9">
         <v>122</v>
       </c>
-      <c r="E74" s="10" t="s">
+      <c r="E74" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F74" s="10" t="s">
+      <c r="F74" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="10">
+      <c r="A75" s="9">
         <v>38732</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B75" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="C75" s="10">
+      <c r="C75" s="9">
         <v>3</v>
       </c>
-      <c r="D75" s="10">
+      <c r="D75" s="9">
         <v>122</v>
       </c>
-      <c r="E75" s="10" t="s">
+      <c r="E75" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F75" s="10" t="s">
+      <c r="F75" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="10">
+      <c r="A76" s="9">
         <v>38865</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B76" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="C76" s="10">
+      <c r="C76" s="9">
         <v>3</v>
       </c>
-      <c r="D76" s="10">
+      <c r="D76" s="9">
         <v>122</v>
       </c>
-      <c r="E76" s="10" t="s">
+      <c r="E76" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F76" s="10" t="s">
+      <c r="F76" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="10">
+      <c r="A77" s="9">
         <v>39709</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B77" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="C77" s="10">
+      <c r="C77" s="9">
         <v>3</v>
       </c>
-      <c r="D77" s="10">
+      <c r="D77" s="9">
         <v>122</v>
       </c>
-      <c r="E77" s="10" t="s">
+      <c r="E77" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F77" s="10" t="s">
+      <c r="F77" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="10">
+      <c r="A78" s="9">
         <v>39743</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B78" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="C78" s="10">
+      <c r="C78" s="9">
         <v>3</v>
       </c>
-      <c r="D78" s="10">
+      <c r="D78" s="9">
         <v>122</v>
       </c>
-      <c r="E78" s="10" t="s">
+      <c r="E78" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="F78" s="10" t="s">
+      <c r="F78" s="9" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="10">
+      <c r="A79" s="9">
         <v>41443</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B79" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="C79" s="10">
+      <c r="C79" s="9">
         <v>3</v>
       </c>
-      <c r="D79" s="10">
+      <c r="D79" s="9">
         <v>122</v>
       </c>
-      <c r="E79" s="10" t="s">
+      <c r="E79" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F79" s="10" t="s">
+      <c r="F79" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="10">
+      <c r="A80" s="9">
         <v>47125</v>
       </c>
-      <c r="B80" s="10" t="s">
+      <c r="B80" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="C80" s="10">
+      <c r="C80" s="9">
         <v>3</v>
       </c>
-      <c r="D80" s="10">
+      <c r="D80" s="9">
         <v>150</v>
       </c>
-      <c r="E80" s="10" t="s">
+      <c r="E80" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="F80" s="10" t="s">
+      <c r="F80" s="9" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="10">
+      <c r="A81" s="9">
         <v>47259</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C81" s="10">
+      <c r="C81" s="9">
         <v>3</v>
       </c>
-      <c r="D81" s="10">
+      <c r="D81" s="9">
         <v>150</v>
       </c>
-      <c r="E81" s="10" t="s">
+      <c r="E81" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="F81" s="10" t="s">
+      <c r="F81" s="9" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="10">
+      <c r="A82" s="9">
         <v>47572</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B82" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="C82" s="10">
+      <c r="C82" s="9">
         <v>3</v>
       </c>
-      <c r="D82" s="10">
+      <c r="D82" s="9">
         <v>150</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="E82" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="F82" s="10" t="s">
+      <c r="F82" s="9" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="10">
+      <c r="A83" s="9">
         <v>47618</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B83" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="C83" s="10">
+      <c r="C83" s="9">
         <v>3</v>
       </c>
-      <c r="D83" s="10">
+      <c r="D83" s="9">
         <v>150</v>
       </c>
-      <c r="E83" s="10" t="s">
+      <c r="E83" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="F83" s="9" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="10">
+      <c r="A84" s="9">
         <v>47678</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="C84" s="10">
+      <c r="C84" s="9">
         <v>3</v>
       </c>
-      <c r="D84" s="10">
+      <c r="D84" s="9">
         <v>150</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="E84" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="F84" s="9" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="10">
+      <c r="A85" s="9">
         <v>48183</v>
       </c>
-      <c r="B85" s="10" t="s">
+      <c r="B85" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="C85" s="10">
+      <c r="C85" s="9">
         <v>3</v>
       </c>
-      <c r="D85" s="10">
+      <c r="D85" s="9">
         <v>22</v>
       </c>
-      <c r="E85" s="10" t="s">
+      <c r="E85" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="F85" s="10" t="s">
+      <c r="F85" s="9" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="10">
+      <c r="A86" s="9">
         <v>48303</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B86" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="C86" s="10">
+      <c r="C86" s="9">
         <v>3</v>
       </c>
-      <c r="D86" s="10">
+      <c r="D86" s="9">
         <v>150</v>
       </c>
-      <c r="E86" s="10" t="s">
+      <c r="E86" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="F86" s="10" t="s">
+      <c r="F86" s="9" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="10">
+      <c r="A87" s="9">
         <v>48365</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B87" s="9" t="s">
         <v>344</v>
       </c>
-      <c r="C87" s="10">
+      <c r="C87" s="9">
         <v>3</v>
       </c>
-      <c r="D87" s="10">
+      <c r="D87" s="9">
         <v>150</v>
       </c>
-      <c r="E87" s="10" t="s">
+      <c r="E87" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="F87" s="10" t="s">
+      <c r="F87" s="9" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="10">
+      <c r="A88" s="9">
         <v>48565</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B88" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="C88" s="10">
+      <c r="C88" s="9">
         <v>3</v>
       </c>
-      <c r="D88" s="10">
+      <c r="D88" s="9">
         <v>150</v>
       </c>
-      <c r="E88" s="10" t="s">
+      <c r="E88" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="F88" s="10" t="s">
+      <c r="F88" s="9" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="10">
+      <c r="A89" s="9">
         <v>48816</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B89" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="C89" s="10">
+      <c r="C89" s="9">
         <v>3</v>
       </c>
-      <c r="D89" s="10">
+      <c r="D89" s="9">
         <v>150</v>
       </c>
-      <c r="E89" s="10" t="s">
+      <c r="E89" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="F89" s="10" t="s">
+      <c r="F89" s="9" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="10">
+      <c r="A90" s="9">
         <v>48864</v>
       </c>
-      <c r="B90" s="10" t="s">
+      <c r="B90" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="C90" s="10">
+      <c r="C90" s="9">
         <v>3</v>
       </c>
-      <c r="D90" s="10">
+      <c r="D90" s="9">
         <v>150</v>
       </c>
-      <c r="E90" s="10" t="s">
+      <c r="E90" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="F90" s="10" t="s">
+      <c r="F90" s="9" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="10">
+      <c r="A91" s="9">
         <v>48919</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B91" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="C91" s="10">
+      <c r="C91" s="9">
         <v>3</v>
       </c>
-      <c r="D91" s="10">
+      <c r="D91" s="9">
         <v>150</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="E91" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="F91" s="10" t="s">
+      <c r="F91" s="9" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="10">
+      <c r="A92" s="9">
         <v>48955</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="B92" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="C92" s="10">
+      <c r="C92" s="9">
         <v>3</v>
       </c>
-      <c r="D92" s="10">
+      <c r="D92" s="9">
         <v>150</v>
       </c>
-      <c r="E92" s="10" t="s">
+      <c r="E92" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="F92" s="10" t="s">
+      <c r="F92" s="9" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="10">
+      <c r="A93" s="9">
         <v>49009</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B93" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="C93" s="10">
+      <c r="C93" s="9">
         <v>3</v>
       </c>
-      <c r="D93" s="10">
+      <c r="D93" s="9">
         <v>150</v>
       </c>
-      <c r="E93" s="10" t="s">
+      <c r="E93" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="F93" s="10" t="s">
+      <c r="F93" s="9" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="10">
+      <c r="A94" s="9">
         <v>49039</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B94" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="C94" s="10">
+      <c r="C94" s="9">
         <v>3</v>
       </c>
-      <c r="D94" s="10">
+      <c r="D94" s="9">
         <v>150</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="E94" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="F94" s="9" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="10">
+      <c r="A95" s="9">
         <v>49071</v>
       </c>
-      <c r="B95" s="10" t="s">
+      <c r="B95" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="C95" s="10">
+      <c r="C95" s="9">
         <v>3</v>
       </c>
-      <c r="D95" s="10">
+      <c r="D95" s="9">
         <v>150</v>
       </c>
-      <c r="E95" s="10" t="s">
+      <c r="E95" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="F95" s="10" t="s">
+      <c r="F95" s="9" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="10">
+      <c r="A96" s="9">
         <v>49551</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B96" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="C96" s="10">
+      <c r="C96" s="9">
         <v>3</v>
       </c>
-      <c r="D96" s="10">
+      <c r="D96" s="9">
         <v>2</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="E96" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F96" s="10" t="s">
+      <c r="F96" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="10">
+      <c r="A97" s="9">
         <v>50038</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B97" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="C97" s="10">
+      <c r="C97" s="9">
         <v>3</v>
       </c>
-      <c r="D97" s="10">
+      <c r="D97" s="9">
         <v>150</v>
       </c>
-      <c r="E97" s="10" t="s">
+      <c r="E97" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="F97" s="10" t="s">
+      <c r="F97" s="9" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="10">
+      <c r="A98" s="9">
         <v>51577</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="C98" s="10">
+      <c r="C98" s="9">
         <v>3</v>
       </c>
-      <c r="D98" s="10">
+      <c r="D98" s="9">
         <v>150</v>
       </c>
-      <c r="E98" s="10" t="s">
+      <c r="E98" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="F98" s="10" t="s">
+      <c r="F98" s="9" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="10">
+      <c r="A99" s="9">
         <v>51835</v>
       </c>
-      <c r="B99" s="10" t="s">
+      <c r="B99" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="C99" s="10">
+      <c r="C99" s="9">
         <v>3</v>
       </c>
-      <c r="D99" s="10">
+      <c r="D99" s="9">
         <v>150</v>
       </c>
-      <c r="E99" s="10" t="s">
+      <c r="E99" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="F99" s="10" t="s">
+      <c r="F99" s="9" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="10">
+      <c r="A100" s="9">
         <v>52026</v>
       </c>
-      <c r="B100" s="10" t="s">
+      <c r="B100" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="C100" s="10">
+      <c r="C100" s="9">
         <v>3</v>
       </c>
-      <c r="D100" s="10">
+      <c r="D100" s="9">
         <v>150</v>
       </c>
-      <c r="E100" s="10" t="s">
+      <c r="E100" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="F100" s="10" t="s">
+      <c r="F100" s="9" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="10">
+      <c r="A101" s="9">
         <v>52459</v>
       </c>
-      <c r="B101" s="10" t="s">
+      <c r="B101" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="C101" s="10">
+      <c r="C101" s="9">
         <v>3</v>
       </c>
-      <c r="D101" s="10">
+      <c r="D101" s="9">
         <v>150</v>
       </c>
-      <c r="E101" s="10" t="s">
+      <c r="E101" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="F101" s="10" t="s">
+      <c r="F101" s="9" t="s">
         <v>386</v>
       </c>
     </row>
@@ -6938,22 +6937,22 @@
   <sheetFormatPr defaultColWidth="32.8359375" defaultRowHeight="14" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" ht="17" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>166</v>
       </c>
     </row>
@@ -6996,7 +6995,7 @@
   <dimension ref="A1:P640"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -7018,92 +7017,92 @@
       </c>
     </row>
     <row r="2" ht="16.8" spans="1:3">
-      <c r="A2" s="4">
+      <c r="A2">
         <v>194636</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="3" ht="16.8" spans="1:6">
-      <c r="A3" s="4">
+      <c r="A3">
         <v>138181</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="4" ht="16.8" spans="1:3">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>126167</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="5" ht="16.8" spans="1:3">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>241097</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="17" spans="1:16">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>87773</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>5</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="4" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="7" ht="16.8" spans="1:9">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>120317</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>4</v>
       </c>
       <c r="I7" t="s">
@@ -7111,46 +7110,46 @@
       </c>
     </row>
     <row r="8" ht="16.8" spans="1:3">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>227496</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" ht="16.8" spans="1:3">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>120317</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="10" ht="16.8" spans="1:3">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>223389</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="11" ht="16.8" spans="1:15">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>99962</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>4</v>
       </c>
       <c r="M11">
@@ -7164,13 +7163,13 @@
       </c>
     </row>
     <row r="12" ht="16.8" spans="1:15">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>46923</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>7</v>
       </c>
       <c r="M12">
@@ -7184,13 +7183,13 @@
       </c>
     </row>
     <row r="13" ht="16.8" spans="1:15">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>52814</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>1</v>
       </c>
       <c r="M13">
@@ -7204,13 +7203,13 @@
       </c>
     </row>
     <row r="14" ht="16.8" spans="1:15">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>79618</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>3</v>
       </c>
       <c r="M14">
@@ -7224,13 +7223,13 @@
       </c>
     </row>
     <row r="15" ht="16.8" spans="1:15">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>125952</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="M15">
@@ -7244,13 +7243,13 @@
       </c>
     </row>
     <row r="16" ht="16.8" spans="1:15">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>126301</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="M16">
@@ -7264,13 +7263,13 @@
       </c>
     </row>
     <row r="17" ht="16.8" spans="1:15">
-      <c r="A17" s="4">
+      <c r="A17">
         <v>86430</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>2</v>
       </c>
       <c r="M17">
@@ -7284,13 +7283,13 @@
       </c>
     </row>
     <row r="18" ht="16.8" spans="1:15">
-      <c r="A18" s="4">
+      <c r="A18">
         <v>118357</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>1883</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>1</v>
       </c>
       <c r="M18">
@@ -7304,13 +7303,13 @@
       </c>
     </row>
     <row r="19" ht="16.8" spans="1:15">
-      <c r="A19" s="4">
+      <c r="A19">
         <v>117488</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="M19">
@@ -7324,13 +7323,13 @@
       </c>
     </row>
     <row r="20" ht="16.8" spans="1:15">
-      <c r="A20" s="4">
+      <c r="A20">
         <v>90452</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>1</v>
       </c>
       <c r="M20">
@@ -7344,13 +7343,13 @@
       </c>
     </row>
     <row r="21" ht="16.8" spans="1:15">
-      <c r="A21" s="4">
+      <c r="A21">
         <v>79618</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>2</v>
       </c>
       <c r="M21">
@@ -7364,13 +7363,13 @@
       </c>
     </row>
     <row r="22" ht="16.8" spans="1:15">
-      <c r="A22" s="4">
+      <c r="A22">
         <v>83135</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>2</v>
       </c>
       <c r="M22">
@@ -7384,13 +7383,13 @@
       </c>
     </row>
     <row r="23" ht="16.8" spans="1:15">
-      <c r="A23" s="4">
+      <c r="A23">
         <v>62084</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>5</v>
       </c>
       <c r="M23">
@@ -7404,13 +7403,13 @@
       </c>
     </row>
     <row r="24" ht="16.8" spans="1:15">
-      <c r="A24" s="4">
+      <c r="A24">
         <v>43982</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>5</v>
       </c>
       <c r="M24">
@@ -7424,13 +7423,13 @@
       </c>
     </row>
     <row r="25" ht="16.8" spans="1:15">
-      <c r="A25" s="4">
+      <c r="A25">
         <v>79618</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>1</v>
       </c>
       <c r="M25">
@@ -7444,13 +7443,13 @@
       </c>
     </row>
     <row r="26" ht="16.8" spans="1:15">
-      <c r="A26" s="4">
+      <c r="A26">
         <v>84231</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>1</v>
       </c>
       <c r="M26">
@@ -7464,13 +7463,13 @@
       </c>
     </row>
     <row r="27" ht="16.8" spans="1:15">
-      <c r="A27" s="4">
+      <c r="A27">
         <v>90254</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>1</v>
       </c>
       <c r="M27">
@@ -7484,13 +7483,13 @@
       </c>
     </row>
     <row r="28" ht="16.8" spans="1:15">
-      <c r="A28" s="4">
+      <c r="A28">
         <v>83135</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>1</v>
       </c>
       <c r="M28">
@@ -7504,13 +7503,13 @@
       </c>
     </row>
     <row r="29" ht="16.8" spans="1:15">
-      <c r="A29" s="4">
+      <c r="A29">
         <v>62084</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>4</v>
       </c>
       <c r="M29">
@@ -7524,13 +7523,13 @@
       </c>
     </row>
     <row r="30" ht="16.8" spans="1:15">
-      <c r="A30" s="4">
+      <c r="A30">
         <v>66871</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>2</v>
       </c>
       <c r="M30">
@@ -7544,13 +7543,13 @@
       </c>
     </row>
     <row r="31" ht="16.8" spans="1:15">
-      <c r="A31" s="4">
+      <c r="A31">
         <v>62084</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>3</v>
       </c>
       <c r="M31">
@@ -7564,13 +7563,13 @@
       </c>
     </row>
     <row r="32" ht="16.8" spans="1:15">
-      <c r="A32" s="4">
+      <c r="A32">
         <v>70390</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>1</v>
       </c>
       <c r="M32">
@@ -7584,13 +7583,13 @@
       </c>
     </row>
     <row r="33" ht="16.8" spans="1:15">
-      <c r="A33" s="4">
+      <c r="A33">
         <v>66871</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <v>1</v>
       </c>
       <c r="M33">
@@ -7604,13 +7603,13 @@
       </c>
     </row>
     <row r="34" ht="16.8" spans="1:15">
-      <c r="A34" s="4">
+      <c r="A34">
         <v>43982</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="4">
         <v>4</v>
       </c>
       <c r="M34">
@@ -7624,13 +7623,13 @@
       </c>
     </row>
     <row r="35" ht="16.8" spans="1:15">
-      <c r="A35" s="4">
+      <c r="A35">
         <v>64421</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="4">
         <v>2</v>
       </c>
       <c r="M35">
@@ -7644,13 +7643,13 @@
       </c>
     </row>
     <row r="36" ht="16.8" spans="1:15">
-      <c r="A36" s="4">
+      <c r="A36">
         <v>62425</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="4">
         <v>3</v>
       </c>
       <c r="M36">
@@ -7664,536 +7663,536 @@
       </c>
     </row>
     <row r="37" ht="16.8" spans="1:3">
-      <c r="A37" s="4">
+      <c r="A37">
         <v>56336</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="38" ht="16.8" spans="1:3">
-      <c r="A38" s="4">
+      <c r="A38">
         <v>61239</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="39" ht="16.8" spans="1:3">
-      <c r="A39" s="4">
+      <c r="A39">
         <v>64593</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="40" ht="16.8" spans="1:3">
-      <c r="A40" s="4">
+      <c r="A40">
         <v>46643</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="41" ht="16.8" spans="1:3">
-      <c r="A41" s="4">
+      <c r="A41">
         <v>62084</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="42" ht="16.8" spans="1:3">
-      <c r="A42" s="4">
+      <c r="A42">
         <v>43982</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="43" ht="16.8" spans="1:3">
-      <c r="A43" s="4">
+      <c r="A43">
         <v>62425</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="44" ht="16.8" spans="1:3">
-      <c r="A44" s="4">
+      <c r="A44">
         <v>56336</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="45" ht="16.8" spans="1:3">
-      <c r="A45" s="4">
+      <c r="A45">
         <v>61239</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="46" ht="16.8" spans="1:3">
-      <c r="A46" s="4">
+      <c r="A46">
         <v>47224</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="47" ht="16.8" spans="1:3">
-      <c r="A47" s="4">
+      <c r="A47">
         <v>46643</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="48" ht="16.8" spans="1:3">
-      <c r="A48" s="4">
+      <c r="A48">
         <v>62084</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="49" ht="16.8" spans="1:3">
-      <c r="A49" s="4">
+      <c r="A49">
         <v>67961</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="50" ht="16.8" spans="1:3">
-      <c r="A50" s="4">
+      <c r="A50">
         <v>64421</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="51" ht="16.8" spans="1:3">
-      <c r="A51" s="4">
+      <c r="A51">
         <v>49010</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="52" ht="16.8" spans="1:3">
-      <c r="A52" s="4">
+      <c r="A52">
         <v>62208</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="53" ht="16.8" spans="1:3">
-      <c r="A53" s="4">
+      <c r="A53">
         <v>43020</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>456</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="54" ht="16.8" spans="1:3">
-      <c r="A54" s="4">
+      <c r="A54">
         <v>62425</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="55" ht="16.8" spans="1:3">
-      <c r="A55" s="4">
+      <c r="A55">
         <v>46643</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="56" ht="16.8" spans="1:3">
-      <c r="A56" s="4">
+      <c r="A56">
         <v>43982</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C56" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="57" ht="16.8" spans="1:3">
-      <c r="A57" s="4">
+      <c r="A57">
         <v>49010</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>458</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="58" ht="16.8" spans="1:3">
-      <c r="A58" s="4">
+      <c r="A58">
         <v>46746</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="59" ht="16.8" spans="1:3">
-      <c r="A59" s="4">
+      <c r="A59">
         <v>46511</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C59" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="60" ht="16.8" spans="1:3">
-      <c r="A60" s="4">
+      <c r="A60">
         <v>46643</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C60" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="61" ht="16.8" spans="1:3">
-      <c r="A61" s="4">
+      <c r="A61">
         <v>62717</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="62" ht="16.8" spans="1:3">
-      <c r="A62" s="4">
+      <c r="A62">
         <v>56484</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C62" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="63" ht="16.8" spans="1:3">
-      <c r="A63" s="4">
+      <c r="A63">
         <v>49010</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="64" ht="16.8" spans="1:3">
-      <c r="A64" s="4">
+      <c r="A64">
         <v>46746</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="65" ht="16.8" spans="1:3">
-      <c r="A65" s="4">
+      <c r="A65">
         <v>46511</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="66" ht="16.8" spans="1:3">
-      <c r="A66" s="4">
+      <c r="A66">
         <v>43020</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="67" ht="16.8" spans="1:3">
-      <c r="A67" s="4">
+      <c r="A67">
         <v>56336</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C67" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="68" ht="16.8" spans="1:3">
-      <c r="A68" s="4">
+      <c r="A68">
         <v>43982</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="69" ht="16.8" spans="1:3">
-      <c r="A69" s="4">
+      <c r="A69">
         <v>39718</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C69" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="70" ht="16.8" spans="1:3">
-      <c r="A70" s="4">
+      <c r="A70">
         <v>43020</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C70" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="71" ht="16.8" spans="1:3">
-      <c r="A71" s="4">
+      <c r="A71">
         <v>43020</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C71" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="72" ht="16.8" spans="1:3">
-      <c r="A72" s="4">
+      <c r="A72">
         <v>39718</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C72" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="73" ht="16.8" spans="1:3">
-      <c r="A73" s="4">
+      <c r="A73">
         <v>4046</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="74" ht="16.8" spans="1:3">
-      <c r="A74" s="4">
+      <c r="A74">
         <v>4046</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="75" ht="16.8" spans="1:3">
-      <c r="A75" s="4">
+      <c r="A75">
         <v>28379</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="76" ht="16.8" spans="1:3">
-      <c r="A76" s="4">
+      <c r="A76">
         <v>4046</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="77" ht="16.8" spans="1:3">
-      <c r="A77" s="4">
+      <c r="A77">
         <v>4046</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C77" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="78" ht="16.8" spans="1:3">
-      <c r="A78" s="4">
+      <c r="A78">
         <v>4046</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C78" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="79" ht="16.8" spans="1:3">
-      <c r="A79" s="4">
+      <c r="A79">
         <v>4046</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="80" ht="16.8" spans="1:3">
-      <c r="A80" s="4">
+      <c r="A80">
         <v>4046</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="81" ht="16.8" spans="1:3">
-      <c r="A81" s="4">
+      <c r="A81">
         <v>4046</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C81" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="82" ht="16.8" spans="1:3">
-      <c r="A82" s="4">
+      <c r="A82">
         <v>4046</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C82" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="83" ht="16.8" spans="1:3">
-      <c r="A83" s="4">
+      <c r="A83">
         <v>4046</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C83" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="84" ht="16.8" spans="1:3">
-      <c r="A84" s="9">
+      <c r="A84">
         <v>39718</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="C84" s="9">
+      <c r="C84" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="85" ht="16.8" spans="1:15">
       <c r="A85"/>
-      <c r="O85" s="7" t="s">
+      <c r="O85" s="6" t="s">
         <v>481</v>
       </c>
     </row>

</xml_diff>